<commit_message>
Rename semiLightIntense to manuLightIntense
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shibin.hoo\Documents\GitHub\Ellemento\rack_control\variable_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shibin.hoo\Documents\GitHub\Ellemento\rack_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="15120" windowHeight="14220"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="15120" windowHeight="14220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="437">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1193,9 +1193,6 @@
     <t>k_shelf_semiLightOnIndexOffset</t>
   </si>
   <si>
-    <t>k_shelf_semiLightIntensIndexOffset</t>
-  </si>
-  <si>
     <t>k_shelf_manuPvPosIndexOffset</t>
   </si>
   <si>
@@ -1226,9 +1223,6 @@
     <t>offset from shelf_x_addr to get shelf_x_semiLightOn</t>
   </si>
   <si>
-    <t>offset from shelf_x_addr to get shelf_x_semiLightIntens</t>
-  </si>
-  <si>
     <t>offset from shelf_x_addr to get shelf_x_manuPVPos</t>
   </si>
   <si>
@@ -1262,9 +1256,6 @@
     <t>semiPVOn</t>
   </si>
   <si>
-    <t>semiLightIntensity</t>
-  </si>
-  <si>
     <t>semiLightOn</t>
   </si>
   <si>
@@ -1347,6 +1338,15 @@
   </si>
   <si>
     <t>maximum number of shelves per section</t>
+  </si>
+  <si>
+    <t>manuLightIntensity</t>
+  </si>
+  <si>
+    <t>k_shelf_manuLightIntensIndexOffset</t>
+  </si>
+  <si>
+    <t>offset from shelf_x_addr to get shelf_x_manuLightIntens</t>
   </si>
 </sst>
 </file>
@@ -1357,16 +1357,8 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1400,15 +1392,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1705,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,7 +1705,7 @@
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1762,7 +1751,7 @@
         <v>133</v>
       </c>
       <c r="G2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1775,7 +1764,7 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f>E2*(COUNTA('Sensor List'!B:B)-1) + (COUNTA('Sensor List'!C:C)-1)</f>
         <v>152</v>
       </c>
@@ -1808,7 +1797,7 @@
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1825,7 +1814,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1842,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1859,12 +1848,12 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1876,7 +1865,7 @@
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1893,7 +1882,7 @@
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1910,12 +1899,12 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>385</v>
+        <v>435</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1927,12 +1916,12 @@
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>396</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1944,12 +1933,12 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1961,178 +1950,201 @@
         <v>10000</v>
       </c>
       <c r="G14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="F15" s="3"/>
+      <c r="D15" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="F15" t="s">
+        <v>133</v>
+      </c>
       <c r="G15" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>422</v>
+      <c r="D16" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="F16" t="s">
+        <v>133</v>
       </c>
       <c r="G16" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="D17" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="F17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G17" t="s">
         <v>422</v>
-      </c>
-      <c r="G17" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>422</v>
+      <c r="D18" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="F18" t="s">
+        <v>133</v>
       </c>
       <c r="G18" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>422</v>
+      <c r="D19" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="F19" t="s">
+        <v>133</v>
       </c>
       <c r="G19" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>422</v>
+      <c r="D20" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="F20" t="s">
+        <v>133</v>
       </c>
       <c r="G20" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>422</v>
+      <c r="D21" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
       </c>
       <c r="G21" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="F22" t="s">
+        <v>133</v>
+      </c>
       <c r="G22" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>1</v>
       </c>
       <c r="E23">
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>1</v>
       </c>
       <c r="E24">
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -2144,8 +2156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,16 +2218,16 @@
         <v>133</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="9" t="s">
-        <v>403</v>
+      <c r="I2" s="8" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -2223,7 +2235,7 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>131</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -2232,7 +2244,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -2240,7 +2252,7 @@
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>131</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -2249,7 +2261,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -2266,7 +2278,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -2284,7 +2296,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -2302,7 +2314,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>408</v>
+        <v>434</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -2320,7 +2332,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -2338,7 +2350,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -2353,7 +2365,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -2368,7 +2380,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -3212,7 +3224,7 @@
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -3226,7 +3238,7 @@
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" t="s">
@@ -3241,7 +3253,7 @@
       <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" t="s">
@@ -3255,7 +3267,7 @@
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>1</v>
       </c>
       <c r="D5" t="s">
@@ -3269,7 +3281,7 @@
       <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" t="s">
@@ -3283,7 +3295,7 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
@@ -3294,7 +3306,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="8"/>
+      <c r="C8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3550,7 +3562,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -4491,7 +4503,7 @@
       <c r="C64" t="s">
         <v>3</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4505,7 +4517,7 @@
       <c r="C65" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4519,7 +4531,7 @@
       <c r="C66" t="s">
         <v>3</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4533,7 +4545,7 @@
       <c r="C67" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4547,7 +4559,7 @@
       <c r="C68" t="s">
         <v>3</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4561,7 +4573,7 @@
       <c r="C69" t="s">
         <v>3</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4575,7 +4587,7 @@
       <c r="C70" t="s">
         <v>3</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4589,7 +4601,7 @@
       <c r="C71" t="s">
         <v>3</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4603,7 +4615,7 @@
       <c r="C72" t="s">
         <v>3</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4617,7 +4629,7 @@
       <c r="C73" t="s">
         <v>3</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4631,7 +4643,7 @@
       <c r="C74" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4645,7 +4657,7 @@
       <c r="C75" t="s">
         <v>3</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4659,7 +4671,7 @@
       <c r="C76" t="s">
         <v>3</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4673,7 +4685,7 @@
       <c r="C77" t="s">
         <v>3</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4687,7 +4699,7 @@
       <c r="C78" t="s">
         <v>3</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -5171,7 +5183,7 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -5183,7 +5195,7 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -5195,7 +5207,7 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -5207,7 +5219,7 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -5219,7 +5231,7 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -5231,7 +5243,7 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -5243,7 +5255,7 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -5280,7 +5292,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C12" t="s">
         <v>145</v>
@@ -5291,7 +5303,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C13" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
Create LookUpTableUI and add scheduler for each shelf
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="535">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1229,12 +1229,6 @@
     <t>pump_flowrateFeedback</t>
   </si>
   <si>
-    <t>S0_LOCK_SEMI_PART</t>
-  </si>
-  <si>
-    <t>S0_LOCK_MANU_PART</t>
-  </si>
-  <si>
     <t>k_shelf_baseAddr</t>
   </si>
   <si>
@@ -1629,6 +1623,24 @@
   </si>
   <si>
     <t>S9_PLC_ADDR_OFFSET</t>
+  </si>
+  <si>
+    <t>SEC0_LOCK_SEMI_PART</t>
+  </si>
+  <si>
+    <t>SEC0_LOCK_MANU_PART</t>
+  </si>
+  <si>
+    <t>SEC1_LOCK_SEMI_PART</t>
+  </si>
+  <si>
+    <t>SEC1_LOCK_MANU_PART</t>
+  </si>
+  <si>
+    <t>SEC2_LOCK_SEMI_PART</t>
+  </si>
+  <si>
+    <t>SEC2_LOCK_MANU_PART</t>
   </si>
 </sst>
 </file>
@@ -2189,7 +2201,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2201,7 +2213,7 @@
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2223,7 +2235,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2235,152 +2247,152 @@
         <v>10000</v>
       </c>
       <c r="G14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F15" t="s">
         <v>133</v>
       </c>
       <c r="G15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F16" t="s">
         <v>133</v>
       </c>
       <c r="G16" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F17" t="s">
         <v>133</v>
       </c>
       <c r="G17" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F18" t="s">
         <v>133</v>
       </c>
       <c r="G18" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F19" t="s">
         <v>133</v>
       </c>
       <c r="G19" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F20" t="s">
         <v>133</v>
       </c>
       <c r="G20" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F21" t="s">
         <v>133</v>
       </c>
       <c r="G21" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -2395,12 +2407,12 @@
         <v>133</v>
       </c>
       <c r="G22" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2412,12 +2424,12 @@
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2429,7 +2441,7 @@
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -2503,16 +2515,16 @@
         <v>133</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -2529,7 +2541,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -2546,7 +2558,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -2563,7 +2575,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -2581,7 +2593,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -2599,7 +2611,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -2617,7 +2629,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -2635,7 +2647,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -2650,7 +2662,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -2665,7 +2677,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -5424,10 +5436,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5578,7 +5590,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>397</v>
+        <v>529</v>
       </c>
       <c r="C12" t="s">
         <v>145</v>
@@ -5589,7 +5601,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>398</v>
+        <v>530</v>
       </c>
       <c r="C13" t="s">
         <v>145</v>
@@ -5600,21 +5612,21 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>445</v>
+        <v>531</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>446</v>
+        <v>532</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -5622,10 +5634,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>520</v>
+        <v>533</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -5633,10 +5645,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>519</v>
+        <v>534</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -5644,18 +5656,18 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -5666,7 +5678,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>439</v>
+        <v>518</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -5677,7 +5689,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>440</v>
+        <v>517</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -5688,7 +5700,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -5699,7 +5711,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -5710,7 +5722,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
@@ -5721,7 +5733,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -5732,7 +5744,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -5743,7 +5755,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -5754,7 +5766,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -5765,7 +5777,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -5776,7 +5788,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -5787,7 +5799,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -5798,7 +5810,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
@@ -5809,7 +5821,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -5820,7 +5832,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -5831,7 +5843,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -5842,7 +5854,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -5853,7 +5865,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -5864,7 +5876,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
@@ -5875,7 +5887,7 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
@@ -5886,7 +5898,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -5897,7 +5909,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
@@ -5908,7 +5920,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -5919,7 +5931,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -5930,7 +5942,7 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
@@ -5941,7 +5953,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
@@ -5952,7 +5964,7 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
@@ -5963,7 +5975,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
@@ -5974,7 +5986,7 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
@@ -5985,7 +5997,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
@@ -5996,7 +6008,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
@@ -6007,7 +6019,7 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
@@ -6018,7 +6030,7 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -6029,7 +6041,7 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
@@ -6040,7 +6052,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
@@ -6051,7 +6063,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
@@ -6062,7 +6074,7 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
@@ -6073,7 +6085,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
@@ -6084,7 +6096,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
@@ -6095,7 +6107,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -6106,7 +6118,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
@@ -6117,7 +6129,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
@@ -6128,7 +6140,7 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
@@ -6139,7 +6151,7 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
@@ -6150,7 +6162,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
@@ -6161,7 +6173,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
@@ -6172,7 +6184,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
@@ -6183,7 +6195,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
@@ -6194,7 +6206,7 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
@@ -6205,7 +6217,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
@@ -6216,7 +6228,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
@@ -6227,7 +6239,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
@@ -6238,7 +6250,7 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
@@ -6249,7 +6261,7 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
@@ -6260,7 +6272,7 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
@@ -6271,7 +6283,7 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
@@ -6282,7 +6294,7 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
@@ -6293,7 +6305,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
@@ -6304,7 +6316,7 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
@@ -6315,7 +6327,7 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
@@ -6326,7 +6338,7 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
@@ -6337,7 +6349,7 @@
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
@@ -6348,7 +6360,7 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
@@ -6359,7 +6371,7 @@
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
@@ -6370,7 +6382,7 @@
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
@@ -6381,7 +6393,7 @@
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
@@ -6392,7 +6404,7 @@
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
@@ -6403,7 +6415,7 @@
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
@@ -6414,7 +6426,7 @@
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
@@ -6425,7 +6437,7 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
@@ -6436,7 +6448,7 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
@@ -6447,7 +6459,7 @@
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
@@ -6458,7 +6470,7 @@
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
@@ -6469,7 +6481,7 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
@@ -6480,7 +6492,7 @@
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
@@ -6491,7 +6503,7 @@
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
@@ -6502,7 +6514,7 @@
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
@@ -6513,7 +6525,7 @@
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
@@ -6524,7 +6536,7 @@
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="C98" t="s">
         <v>1</v>
@@ -6535,7 +6547,7 @@
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="C99" t="s">
         <v>1</v>
@@ -6546,7 +6558,7 @@
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
@@ -6557,7 +6569,7 @@
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
@@ -6568,7 +6580,7 @@
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
@@ -6579,7 +6591,7 @@
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
@@ -6590,7 +6602,7 @@
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="C104" t="s">
         <v>1</v>
@@ -6601,7 +6613,7 @@
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C105" t="s">
         <v>1</v>
@@ -6612,7 +6624,7 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
@@ -6623,12 +6635,56 @@
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
       </c>
       <c r="D107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>525</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>526</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>527</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>528</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Debug addr and macro error in UI
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="538">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1641,6 +1641,15 @@
   </si>
   <si>
     <t>SEC2_LOCK_MANU_PART</t>
+  </si>
+  <si>
+    <t>DUMMY_WORD0</t>
+  </si>
+  <si>
+    <t>DUMMY_WORD1</t>
+  </si>
+  <si>
+    <t>DUMMY_WORD2</t>
   </si>
 </sst>
 </file>
@@ -5436,10 +5445,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5557,51 +5566,54 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>150</v>
+        <v>535</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>20</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>375</v>
+        <v>536</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>376</v>
+        <v>537</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>529</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>530</v>
+        <v>375</v>
       </c>
       <c r="C13" t="s">
         <v>145</v>
@@ -5612,7 +5624,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>531</v>
+        <v>376</v>
       </c>
       <c r="C14" t="s">
         <v>145</v>
@@ -5623,7 +5635,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C15" t="s">
         <v>145</v>
@@ -5634,7 +5646,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C16" t="s">
         <v>145</v>
@@ -5645,7 +5657,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C17" t="s">
         <v>145</v>
@@ -5656,21 +5668,21 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>443</v>
+        <v>532</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>444</v>
+        <v>533</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -5678,10 +5690,10 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>518</v>
+        <v>534</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -5689,18 +5701,18 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>517</v>
+        <v>443</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -5711,7 +5723,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>436</v>
+        <v>518</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -5722,7 +5734,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>437</v>
+        <v>517</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
@@ -5733,7 +5745,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -5744,7 +5756,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -5755,7 +5767,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -5766,7 +5778,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -5777,7 +5789,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -5788,7 +5800,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -5799,7 +5811,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -5810,7 +5822,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
@@ -5821,7 +5833,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -5832,7 +5844,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -5843,7 +5855,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -5854,7 +5866,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -5865,7 +5877,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -5876,7 +5888,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
@@ -5887,7 +5899,7 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
@@ -5898,7 +5910,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -5909,7 +5921,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
@@ -5920,7 +5932,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -5931,7 +5943,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -5942,7 +5954,7 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
@@ -5953,7 +5965,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
@@ -5964,7 +5976,7 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
@@ -5975,7 +5987,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
@@ -5986,7 +5998,7 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
@@ -5997,7 +6009,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
@@ -6008,7 +6020,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
@@ -6019,7 +6031,7 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
@@ -6030,7 +6042,7 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -6041,7 +6053,7 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
@@ -6052,7 +6064,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
@@ -6063,7 +6075,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
@@ -6074,7 +6086,7 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
@@ -6085,7 +6097,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
@@ -6096,7 +6108,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
@@ -6107,7 +6119,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -6118,7 +6130,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
@@ -6129,7 +6141,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
@@ -6140,7 +6152,7 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
@@ -6151,7 +6163,7 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
@@ -6162,7 +6174,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
@@ -6173,7 +6185,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
@@ -6184,7 +6196,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
@@ -6195,7 +6207,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
@@ -6206,7 +6218,7 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
@@ -6217,7 +6229,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
@@ -6228,7 +6240,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
@@ -6239,7 +6251,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
@@ -6250,7 +6262,7 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
@@ -6261,7 +6273,7 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
@@ -6272,7 +6284,7 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
@@ -6283,7 +6295,7 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
@@ -6294,7 +6306,7 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
@@ -6305,7 +6317,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
@@ -6316,7 +6328,7 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
@@ -6327,7 +6339,7 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
@@ -6338,7 +6350,7 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
@@ -6349,7 +6361,7 @@
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
@@ -6360,7 +6372,7 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
@@ -6371,7 +6383,7 @@
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
@@ -6382,7 +6394,7 @@
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
@@ -6393,7 +6405,7 @@
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
@@ -6404,7 +6416,7 @@
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
@@ -6415,7 +6427,7 @@
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
@@ -6426,7 +6438,7 @@
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
@@ -6437,7 +6449,7 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
@@ -6448,7 +6460,7 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
@@ -6459,7 +6471,7 @@
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
@@ -6470,7 +6482,7 @@
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
@@ -6481,7 +6493,7 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
@@ -6492,7 +6504,7 @@
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
@@ -6503,7 +6515,7 @@
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
@@ -6514,7 +6526,7 @@
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
@@ -6525,7 +6537,7 @@
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
@@ -6536,7 +6548,7 @@
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C98" t="s">
         <v>1</v>
@@ -6547,7 +6559,7 @@
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C99" t="s">
         <v>1</v>
@@ -6558,7 +6570,7 @@
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
@@ -6569,7 +6581,7 @@
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
@@ -6580,7 +6592,7 @@
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
@@ -6591,7 +6603,7 @@
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
@@ -6602,7 +6614,7 @@
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="C104" t="s">
         <v>1</v>
@@ -6613,7 +6625,7 @@
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C105" t="s">
         <v>1</v>
@@ -6624,7 +6636,7 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
@@ -6635,7 +6647,7 @@
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
@@ -6646,7 +6658,7 @@
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
@@ -6657,7 +6669,7 @@
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
@@ -6668,7 +6680,7 @@
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C110" t="s">
         <v>1</v>
@@ -6679,12 +6691,45 @@
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
+        <v>525</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>526</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>527</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
         <v>528</v>
       </c>
-      <c r="C111" t="s">
-        <v>1</v>
-      </c>
-      <c r="D111">
+      <c r="C114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D114">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update f_ShelfController, f_ShelfLogicController, and others helpers function.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="15120" windowHeight="14220" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="15120" windowHeight="14220" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="621">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1650,6 +1650,255 @@
   </si>
   <si>
     <t>DUMMY_WORD2</t>
+  </si>
+  <si>
+    <t>manuLightOn</t>
+  </si>
+  <si>
+    <t>k_shelf_manuLightOnIndexOffset</t>
+  </si>
+  <si>
+    <t>offset from shelf_x_addr to get shelf_x_manuLightOn</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_0</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_1</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_2</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_3</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_4</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_5</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_6</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_7</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_8</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_9</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_10</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_11</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_12</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_13</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_14</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_15</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_16</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_17</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_18</t>
+  </si>
+  <si>
+    <t>IO_waterTemp_19</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_0</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_1</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_2</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_3</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_4</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_5</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_6</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_7</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_8</t>
+  </si>
+  <si>
+    <t>IO_lightIntensity_9</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_0</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_1</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_2</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_3</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_4</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_5</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_6</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_7</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_8</t>
+  </si>
+  <si>
+    <t>IO_lightOnOff_9</t>
+  </si>
+  <si>
+    <t>D28302</t>
+  </si>
+  <si>
+    <t>D28304</t>
+  </si>
+  <si>
+    <t>D28306</t>
+  </si>
+  <si>
+    <t>D28308</t>
+  </si>
+  <si>
+    <t>D28310</t>
+  </si>
+  <si>
+    <t>D28312</t>
+  </si>
+  <si>
+    <t>D28314</t>
+  </si>
+  <si>
+    <t>D28316</t>
+  </si>
+  <si>
+    <t>D28322</t>
+  </si>
+  <si>
+    <t>D28324</t>
+  </si>
+  <si>
+    <t>D28326</t>
+  </si>
+  <si>
+    <t>D28328</t>
+  </si>
+  <si>
+    <t>D28330</t>
+  </si>
+  <si>
+    <t>D28332</t>
+  </si>
+  <si>
+    <t>D28334</t>
+  </si>
+  <si>
+    <t>D28336</t>
+  </si>
+  <si>
+    <t>D28342</t>
+  </si>
+  <si>
+    <t>D28344</t>
+  </si>
+  <si>
+    <t>D28346</t>
+  </si>
+  <si>
+    <t>D28348</t>
+  </si>
+  <si>
+    <t>D28362</t>
+  </si>
+  <si>
+    <t>D28364</t>
+  </si>
+  <si>
+    <t>D28366</t>
+  </si>
+  <si>
+    <t>D28368</t>
+  </si>
+  <si>
+    <t>D28382</t>
+  </si>
+  <si>
+    <t>D28384</t>
+  </si>
+  <si>
+    <t>D28386</t>
+  </si>
+  <si>
+    <t>D28388</t>
+  </si>
+  <si>
+    <t>D28402</t>
+  </si>
+  <si>
+    <t>D28404</t>
+  </si>
+  <si>
+    <t>D28420.0</t>
+  </si>
+  <si>
+    <t>D28420.1</t>
+  </si>
+  <si>
+    <t>D28420.2</t>
+  </si>
+  <si>
+    <t>D28420.3</t>
+  </si>
+  <si>
+    <t>D28420.4</t>
+  </si>
+  <si>
+    <t>D28420.5</t>
+  </si>
+  <si>
+    <t>D28420.6</t>
+  </si>
+  <si>
+    <t>D28420.7</t>
+  </si>
+  <si>
+    <t>D28421.0</t>
+  </si>
+  <si>
+    <t>D28421.1</t>
   </si>
 </sst>
 </file>
@@ -1995,10 +2244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,7 +2459,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>433</v>
+        <v>539</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2222,12 +2471,12 @@
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>434</v>
+        <v>540</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>385</v>
+        <v>433</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2239,12 +2488,12 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>395</v>
+        <v>434</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2253,35 +2502,32 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>10000</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="F15" t="s">
-        <v>133</v>
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>10000</v>
       </c>
       <c r="G15" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -2296,12 +2542,12 @@
         <v>133</v>
       </c>
       <c r="G16" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -2316,12 +2562,12 @@
         <v>133</v>
       </c>
       <c r="G17" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -2336,12 +2582,12 @@
         <v>133</v>
       </c>
       <c r="G18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -2356,12 +2602,12 @@
         <v>133</v>
       </c>
       <c r="G19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -2376,12 +2622,12 @@
         <v>133</v>
       </c>
       <c r="G20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -2396,60 +2642,80 @@
         <v>133</v>
       </c>
       <c r="G21" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>11</v>
+        <v>409</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>12</v>
+        <v>417</v>
       </c>
       <c r="F22" t="s">
         <v>133</v>
       </c>
       <c r="G22" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>133</v>
       </c>
       <c r="G23" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>428</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>430</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25">
         <v>4</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" t="s">
         <v>431</v>
       </c>
     </row>
@@ -2460,10 +2726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,15 +2886,15 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>432</v>
+        <v>538</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -2638,7 +2904,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>405</v>
+        <v>432</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -2646,7 +2912,7 @@
       <c r="D9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -2656,7 +2922,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -2667,11 +2933,14 @@
       <c r="E10" s="2">
         <v>0</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -2686,7 +2955,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -2700,6 +2969,18 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>408</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2712,11 +2993,7 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
@@ -2783,6 +3060,10 @@
     </row>
     <row r="27" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
     </row>
     <row r="28" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
@@ -2915,6 +3196,9 @@
     </row>
     <row r="71" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3897,10 +4181,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F108"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117:B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5011,10 +5295,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>307</v>
+        <v>541</v>
       </c>
       <c r="B79" t="s">
-        <v>308</v>
+        <v>581</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
@@ -5025,416 +5309,976 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>542</v>
+      </c>
+      <c r="B80" t="s">
+        <v>582</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>543</v>
+      </c>
+      <c r="B81" t="s">
+        <v>583</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>544</v>
+      </c>
+      <c r="B82" t="s">
+        <v>584</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>545</v>
+      </c>
+      <c r="B83" t="s">
+        <v>585</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>546</v>
+      </c>
+      <c r="B84" t="s">
+        <v>586</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>547</v>
+      </c>
+      <c r="B85" t="s">
+        <v>587</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>548</v>
+      </c>
+      <c r="B86" t="s">
+        <v>588</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>549</v>
+      </c>
+      <c r="B87" t="s">
+        <v>589</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>550</v>
+      </c>
+      <c r="B88" t="s">
+        <v>590</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>551</v>
+      </c>
+      <c r="B89" t="s">
+        <v>591</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>552</v>
+      </c>
+      <c r="B90" t="s">
+        <v>592</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>553</v>
+      </c>
+      <c r="B91" t="s">
+        <v>593</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>554</v>
+      </c>
+      <c r="B92" t="s">
+        <v>594</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>555</v>
+      </c>
+      <c r="B93" t="s">
+        <v>595</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>556</v>
+      </c>
+      <c r="B94" t="s">
+        <v>596</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>557</v>
+      </c>
+      <c r="B95" t="s">
+        <v>597</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>558</v>
+      </c>
+      <c r="B96" t="s">
+        <v>598</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>559</v>
+      </c>
+      <c r="B97" t="s">
+        <v>599</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>560</v>
+      </c>
+      <c r="B98" t="s">
+        <v>600</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>561</v>
+      </c>
+      <c r="B99" t="s">
+        <v>601</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>562</v>
+      </c>
+      <c r="B100" t="s">
+        <v>602</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>563</v>
+      </c>
+      <c r="B101" t="s">
+        <v>603</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>564</v>
+      </c>
+      <c r="B102" t="s">
+        <v>604</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>565</v>
+      </c>
+      <c r="B103" t="s">
+        <v>605</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>566</v>
+      </c>
+      <c r="B104" t="s">
+        <v>606</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>567</v>
+      </c>
+      <c r="B105" t="s">
+        <v>607</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>568</v>
+      </c>
+      <c r="B106" t="s">
+        <v>608</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>569</v>
+      </c>
+      <c r="B107" t="s">
+        <v>609</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>570</v>
+      </c>
+      <c r="B108" t="s">
+        <v>610</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>571</v>
+      </c>
+      <c r="B109" t="s">
+        <v>611</v>
+      </c>
+      <c r="C109" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>572</v>
+      </c>
+      <c r="B110" t="s">
+        <v>612</v>
+      </c>
+      <c r="C110" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>573</v>
+      </c>
+      <c r="B111" t="s">
+        <v>613</v>
+      </c>
+      <c r="C111" t="s">
+        <v>3</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>574</v>
+      </c>
+      <c r="B112" t="s">
+        <v>614</v>
+      </c>
+      <c r="C112" t="s">
+        <v>3</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>575</v>
+      </c>
+      <c r="B113" t="s">
+        <v>615</v>
+      </c>
+      <c r="C113" t="s">
+        <v>3</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>576</v>
+      </c>
+      <c r="B114" t="s">
+        <v>616</v>
+      </c>
+      <c r="C114" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>577</v>
+      </c>
+      <c r="B115" t="s">
+        <v>617</v>
+      </c>
+      <c r="C115" t="s">
+        <v>3</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>578</v>
+      </c>
+      <c r="B116" t="s">
+        <v>618</v>
+      </c>
+      <c r="C116" t="s">
+        <v>3</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>579</v>
+      </c>
+      <c r="B117" t="s">
+        <v>619</v>
+      </c>
+      <c r="C117" t="s">
+        <v>3</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>580</v>
+      </c>
+      <c r="B118" t="s">
+        <v>620</v>
+      </c>
+      <c r="C118" t="s">
+        <v>3</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>307</v>
+      </c>
+      <c r="B119" t="s">
+        <v>308</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>309</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B120" t="s">
         <v>310</v>
       </c>
-      <c r="C80" t="s">
-        <v>1</v>
-      </c>
-      <c r="D80">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="C120" t="s">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>311</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B121" t="s">
         <v>324</v>
       </c>
-      <c r="C81" t="s">
-        <v>1</v>
-      </c>
-      <c r="D81">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="C121" t="s">
+        <v>1</v>
+      </c>
+      <c r="D121">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>313</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B122" t="s">
         <v>325</v>
       </c>
-      <c r="C82" t="s">
-        <v>1</v>
-      </c>
-      <c r="D82">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="C122" t="s">
+        <v>1</v>
+      </c>
+      <c r="D122">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>315</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B123" t="s">
         <v>326</v>
       </c>
-      <c r="C83" t="s">
-        <v>1</v>
-      </c>
-      <c r="D83">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="C123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>317</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B124" t="s">
         <v>327</v>
       </c>
-      <c r="C84" t="s">
-        <v>1</v>
-      </c>
-      <c r="D84">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="C124" t="s">
+        <v>1</v>
+      </c>
+      <c r="D124">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>319</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B125" t="s">
         <v>320</v>
       </c>
-      <c r="C85" t="s">
-        <v>1</v>
-      </c>
-      <c r="D85">
-        <v>-1</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="C125" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125">
+        <v>-1</v>
+      </c>
+      <c r="E125" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>321</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B126" t="s">
         <v>328</v>
       </c>
-      <c r="C86" t="s">
-        <v>1</v>
-      </c>
-      <c r="D86">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="C126" t="s">
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>322</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B127" t="s">
         <v>329</v>
       </c>
-      <c r="C87" t="s">
-        <v>1</v>
-      </c>
-      <c r="D87">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="C127" t="s">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>323</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B128" t="s">
         <v>330</v>
       </c>
-      <c r="C88" t="s">
-        <v>1</v>
-      </c>
-      <c r="D88">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="C128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D128">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>331</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B129" t="s">
         <v>312</v>
       </c>
-      <c r="C89" t="s">
-        <v>1</v>
-      </c>
-      <c r="D89">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="C129" t="s">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>332</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B130" t="s">
         <v>314</v>
       </c>
-      <c r="C90" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="C130" t="s">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>333</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B131" t="s">
         <v>351</v>
       </c>
-      <c r="C91" t="s">
-        <v>1</v>
-      </c>
-      <c r="D91">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="C131" t="s">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>334</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B132" t="s">
         <v>316</v>
       </c>
-      <c r="C92" t="s">
-        <v>1</v>
-      </c>
-      <c r="D92">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="C132" t="s">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>335</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B133" t="s">
         <v>318</v>
       </c>
-      <c r="C93" t="s">
-        <v>1</v>
-      </c>
-      <c r="D93">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="C133" t="s">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>336</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B134" t="s">
         <v>352</v>
       </c>
-      <c r="C94" t="s">
-        <v>1</v>
-      </c>
-      <c r="D94">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="C134" t="s">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>337</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B135" t="s">
         <v>353</v>
       </c>
-      <c r="C95" t="s">
-        <v>1</v>
-      </c>
-      <c r="D95">
-        <v>-1</v>
-      </c>
-      <c r="E95" t="s">
+      <c r="C135" t="s">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <v>-1</v>
+      </c>
+      <c r="E135" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>338</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B136" t="s">
         <v>354</v>
       </c>
-      <c r="C96" t="s">
-        <v>1</v>
-      </c>
-      <c r="D96">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="C136" t="s">
+        <v>1</v>
+      </c>
+      <c r="D136">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>339</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B137" t="s">
         <v>355</v>
       </c>
-      <c r="C97" t="s">
-        <v>1</v>
-      </c>
-      <c r="D97">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="C137" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>340</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B138" t="s">
         <v>356</v>
       </c>
-      <c r="C98" t="s">
-        <v>1</v>
-      </c>
-      <c r="D98">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="C138" t="s">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>341</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B139" t="s">
         <v>357</v>
       </c>
-      <c r="C99" t="s">
-        <v>1</v>
-      </c>
-      <c r="D99">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="C139" t="s">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>342</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B140" t="s">
         <v>358</v>
       </c>
-      <c r="C100" t="s">
-        <v>1</v>
-      </c>
-      <c r="D100">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="C140" t="s">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>343</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B141" t="s">
         <v>359</v>
       </c>
-      <c r="C101" t="s">
-        <v>1</v>
-      </c>
-      <c r="D101">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="C141" t="s">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>344</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B142" t="s">
         <v>360</v>
       </c>
-      <c r="C102" t="s">
-        <v>1</v>
-      </c>
-      <c r="D102">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="C142" t="s">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>345</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B143" t="s">
         <v>361</v>
       </c>
-      <c r="C103" t="s">
-        <v>1</v>
-      </c>
-      <c r="D103">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="C143" t="s">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>346</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B144" t="s">
         <v>362</v>
       </c>
-      <c r="C104" t="s">
-        <v>1</v>
-      </c>
-      <c r="D104">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="C144" t="s">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>347</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B145" t="s">
         <v>363</v>
       </c>
-      <c r="C105" t="s">
-        <v>1</v>
-      </c>
-      <c r="D105">
-        <v>-1</v>
-      </c>
-      <c r="E105" t="s">
+      <c r="C145" t="s">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <v>-1</v>
+      </c>
+      <c r="E145" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>348</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B146" t="s">
         <v>364</v>
       </c>
-      <c r="C106" t="s">
-        <v>1</v>
-      </c>
-      <c r="D106">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="C146" t="s">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>349</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B147" t="s">
         <v>365</v>
       </c>
-      <c r="C107" t="s">
-        <v>1</v>
-      </c>
-      <c r="D107">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="C147" t="s">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>350</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B148" t="s">
         <v>366</v>
       </c>
-      <c r="C108" t="s">
-        <v>1</v>
-      </c>
-      <c r="D108">
+      <c r="C148" t="s">
+        <v>1</v>
+      </c>
+      <c r="D148">
         <v>-1</v>
       </c>
     </row>
@@ -5447,7 +6291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Debug ShelfController (in simulator)
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="15120" windowHeight="14220" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="15120" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -2246,8 +2246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,7 +2346,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>133</v>
@@ -2729,7 +2729,7 @@
   <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4183,7 +4183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B117" sqref="B117:B118"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add PumpStateTransitionManager and ShelfModeToPumpModeManager
ShelfModeToPumpMode: When any shelf mode is changed to manual, pump mode is automatically triggered to manual-FR (for the first instance only)
PumpStateTransition: Smooth transition of running settings between pump modes
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10575" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="635">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1919,15 +1919,6 @@
     <t>whether to enable pump redundancy</t>
   </si>
   <si>
-    <t>pump_ctrlModeFbk</t>
-  </si>
-  <si>
-    <t>pump_runningFbk</t>
-  </si>
-  <si>
-    <t>pump_flowrateFbk</t>
-  </si>
-  <si>
     <t>secPvCountArr[0]: number of PV to turn on in section 0</t>
   </si>
   <si>
@@ -1938,6 +1929,18 @@
   </si>
   <si>
     <t>1 - Flow, 2 - RPM</t>
+  </si>
+  <si>
+    <t>pump_ctrlModeFbkArr</t>
+  </si>
+  <si>
+    <t>pump_runningFbkArr</t>
+  </si>
+  <si>
+    <t>pump_flowrateFbkArr</t>
+  </si>
+  <si>
+    <t>pump_rpmFbkArr</t>
   </si>
 </sst>
 </file>
@@ -2726,7 +2729,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -2738,7 +2741,7 @@
         <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -3998,7 +4001,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4088,12 +4091,12 @@
         <v>133</v>
       </c>
       <c r="G4" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -4178,7 +4181,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -4195,7 +4198,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -4212,7 +4215,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -4228,8 +4231,21 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="B13" t="s">
+        <v>634</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>

</xml_diff>

<commit_message>
Make flowratePerShelf configurable at HMI
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="635">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1907,9 +1907,6 @@
     <t>D25501</t>
   </si>
   <si>
-    <t>k_flowratePerShelf</t>
-  </si>
-  <si>
     <t>flowrate per shelf in lpm</t>
   </si>
   <si>
@@ -1941,6 +1938,9 @@
   </si>
   <si>
     <t>pump_rpmFbkArr</t>
+  </si>
+  <si>
+    <t>flowratePerShelf</t>
   </si>
 </sst>
 </file>
@@ -2288,8 +2288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2729,7 +2729,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -2741,7 +2741,7 @@
         <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -2780,7 +2780,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>623</v>
+        <v>634</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2791,13 +2791,16 @@
       <c r="E27">
         <v>32</v>
       </c>
+      <c r="F27" t="s">
+        <v>133</v>
+      </c>
       <c r="G27" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2809,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>
@@ -4000,7 +4003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -4091,12 +4094,12 @@
         <v>133</v>
       </c>
       <c r="G4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -4181,7 +4184,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -4198,7 +4201,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -4215,7 +4218,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -4232,7 +4235,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C13">
         <v>3</v>

</xml_diff>

<commit_message>
Merged with PV sequence manager code Fix variable generator script
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shibin.hoo\Documents\GitHub\Ellemento\rack_control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\repo\Ellemento\rack_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="652">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1941,6 +1941,57 @@
   </si>
   <si>
     <t>flowratePerShelf</t>
+  </si>
+  <si>
+    <t>main_current_state</t>
+  </si>
+  <si>
+    <t>ARRAY [4] OF INT</t>
+  </si>
+  <si>
+    <t>main_next_state</t>
+  </si>
+  <si>
+    <t>transition_current_state</t>
+  </si>
+  <si>
+    <t>transition_next_state</t>
+  </si>
+  <si>
+    <t>PVChangeMode</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>delay_counter</t>
+  </si>
+  <si>
+    <t>lastPVvalue</t>
+  </si>
+  <si>
+    <t>ARRAY [10] OF REAL</t>
+  </si>
+  <si>
+    <t>Main state machine current state (for each instance)</t>
+  </si>
+  <si>
+    <t>Main state machine next state (for each instance)</t>
+  </si>
+  <si>
+    <t>PV transition state machine current state (for each instance)</t>
+  </si>
+  <si>
+    <t>PV transition state machine next state (for each instance)</t>
+  </si>
+  <si>
+    <t>Counter for delays</t>
+  </si>
+  <si>
+    <t>Store last PV value for comparison whether to run PV change sequence or not</t>
+  </si>
+  <si>
+    <t>[10(0.0)]</t>
   </si>
 </sst>
 </file>
@@ -2286,23 +2337,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2325,7 +2376,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20000</v>
       </c>
@@ -2348,7 +2399,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>25</v>
       </c>
@@ -2363,7 +2414,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -2377,7 +2428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>352</v>
       </c>
@@ -2397,7 +2448,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>353</v>
       </c>
@@ -2414,7 +2465,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>354</v>
       </c>
@@ -2431,7 +2482,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>355</v>
       </c>
@@ -2448,7 +2499,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>359</v>
       </c>
@@ -2465,7 +2516,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>356</v>
       </c>
@@ -2482,7 +2533,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>357</v>
       </c>
@@ -2499,7 +2550,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>501</v>
       </c>
@@ -2516,7 +2567,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>405</v>
       </c>
@@ -2533,7 +2584,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>358</v>
       </c>
@@ -2550,7 +2601,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>369</v>
       </c>
@@ -2567,7 +2618,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>383</v>
       </c>
@@ -2587,7 +2638,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>384</v>
       </c>
@@ -2607,7 +2658,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>385</v>
       </c>
@@ -2627,7 +2678,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>386</v>
       </c>
@@ -2647,7 +2698,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>382</v>
       </c>
@@ -2667,7 +2718,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>387</v>
       </c>
@@ -2687,7 +2738,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>388</v>
       </c>
@@ -2707,7 +2758,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>399</v>
       </c>
@@ -2727,7 +2778,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>627</v>
       </c>
@@ -2744,7 +2795,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>400</v>
       </c>
@@ -2761,7 +2812,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>402</v>
       </c>
@@ -2778,7 +2829,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>634</v>
       </c>
@@ -2798,7 +2849,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>624</v>
       </c>
@@ -2813,6 +2864,122 @@
       </c>
       <c r="G28" t="s">
         <v>625</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>635</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>636</v>
+      </c>
+      <c r="E29" t="s">
+        <v>389</v>
+      </c>
+      <c r="G29" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>637</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>636</v>
+      </c>
+      <c r="E30" t="s">
+        <v>389</v>
+      </c>
+      <c r="G30" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>638</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>636</v>
+      </c>
+      <c r="E31" t="s">
+        <v>389</v>
+      </c>
+      <c r="G31" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>639</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>636</v>
+      </c>
+      <c r="E32" t="s">
+        <v>389</v>
+      </c>
+      <c r="G32" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>640</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>641</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>642</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>381</v>
+      </c>
+      <c r="E34" t="s">
+        <v>389</v>
+      </c>
+      <c r="G34" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>643</v>
+      </c>
+      <c r="C35">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>644</v>
+      </c>
+      <c r="E35" t="s">
+        <v>651</v>
+      </c>
+      <c r="G35" t="s">
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -2828,22 +2995,22 @@
       <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1"/>
-    <col min="7" max="7" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2866,7 +3033,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -2893,7 +3060,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>372</v>
       </c>
@@ -2910,7 +3077,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>373</v>
       </c>
@@ -2927,7 +3094,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>374</v>
       </c>
@@ -2944,7 +3111,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>375</v>
       </c>
@@ -2962,7 +3129,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>376</v>
       </c>
@@ -2980,7 +3147,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>500</v>
       </c>
@@ -2998,7 +3165,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>404</v>
       </c>
@@ -3016,7 +3183,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>377</v>
       </c>
@@ -3034,7 +3201,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>378</v>
       </c>
@@ -3049,7 +3216,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>379</v>
       </c>
@@ -3064,7 +3231,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>380</v>
       </c>
@@ -3079,221 +3246,221 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E18" s="1"/>
       <c r="G18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E19" s="1"/>
       <c r="G19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E20" s="1"/>
       <c r="G20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E21" s="1"/>
       <c r="G21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E22" s="1"/>
       <c r="G22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E23" s="1"/>
       <c r="G23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E24" s="1"/>
       <c r="G24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E25" s="1"/>
       <c r="G25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E26" s="1"/>
       <c r="G26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E27" s="1"/>
       <c r="G27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="1"/>
     </row>
   </sheetData>
@@ -3310,14 +3477,14 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -3328,7 +3495,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>12000</v>
       </c>
@@ -3339,7 +3506,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -3347,7 +3514,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -3355,7 +3522,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -3363,7 +3530,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -3371,487 +3538,487 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" t="s">
         <v>129</v>
       </c>
@@ -3870,17 +4037,17 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -3903,7 +4070,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>350</v>
       </c>
@@ -3920,7 +4087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -3935,7 +4102,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -3949,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -3963,7 +4130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -3977,7 +4144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -3991,7 +4158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
     </row>
   </sheetData>
@@ -4007,17 +4174,17 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.28515625" customWidth="1"/>
+    <col min="7" max="7" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -4040,7 +4207,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>11000</v>
       </c>
@@ -4060,7 +4227,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>138</v>
       </c>
@@ -4077,7 +4244,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>137</v>
       </c>
@@ -4097,7 +4264,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>628</v>
       </c>
@@ -4114,7 +4281,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>139</v>
       </c>
@@ -4131,7 +4298,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>345</v>
       </c>
@@ -4148,7 +4315,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>140</v>
       </c>
@@ -4165,7 +4332,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>141</v>
       </c>
@@ -4182,7 +4349,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>630</v>
       </c>
@@ -4199,7 +4366,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>631</v>
       </c>
@@ -4216,7 +4383,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>632</v>
       </c>
@@ -4233,7 +4400,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>633</v>
       </c>
@@ -4250,7 +4417,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
     </row>
   </sheetData>
@@ -4266,15 +4433,15 @@
       <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4294,7 +4461,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -4308,7 +4475,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>152</v>
       </c>
@@ -4322,7 +4489,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>153</v>
       </c>
@@ -4336,7 +4503,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -4350,7 +4517,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>157</v>
       </c>
@@ -4364,7 +4531,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>158</v>
       </c>
@@ -4378,7 +4545,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -4392,7 +4559,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -4406,7 +4573,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -4420,7 +4587,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>161</v>
       </c>
@@ -4434,7 +4601,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -4448,7 +4615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -4462,7 +4629,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>163</v>
       </c>
@@ -4476,7 +4643,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>164</v>
       </c>
@@ -4490,7 +4657,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>165</v>
       </c>
@@ -4504,7 +4671,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>166</v>
       </c>
@@ -4518,7 +4685,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>167</v>
       </c>
@@ -4532,7 +4699,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>168</v>
       </c>
@@ -4546,7 +4713,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>169</v>
       </c>
@@ -4560,7 +4727,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>170</v>
       </c>
@@ -4574,7 +4741,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>171</v>
       </c>
@@ -4588,7 +4755,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>172</v>
       </c>
@@ -4602,7 +4769,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>173</v>
       </c>
@@ -4616,7 +4783,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>174</v>
       </c>
@@ -4630,7 +4797,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>176</v>
       </c>
@@ -4644,7 +4811,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>175</v>
       </c>
@@ -4658,7 +4825,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>177</v>
       </c>
@@ -4672,7 +4839,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>178</v>
       </c>
@@ -4686,7 +4853,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>179</v>
       </c>
@@ -4700,7 +4867,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>180</v>
       </c>
@@ -4714,7 +4881,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>211</v>
       </c>
@@ -4728,7 +4895,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>212</v>
       </c>
@@ -4742,7 +4909,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>213</v>
       </c>
@@ -4756,7 +4923,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>214</v>
       </c>
@@ -4770,7 +4937,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>215</v>
       </c>
@@ -4784,7 +4951,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>216</v>
       </c>
@@ -4798,7 +4965,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>217</v>
       </c>
@@ -4812,7 +4979,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>218</v>
       </c>
@@ -4826,7 +4993,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>219</v>
       </c>
@@ -4840,7 +5007,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>220</v>
       </c>
@@ -4854,7 +5021,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>221</v>
       </c>
@@ -4868,7 +5035,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>222</v>
       </c>
@@ -4882,7 +5049,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>223</v>
       </c>
@@ -4896,7 +5063,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>224</v>
       </c>
@@ -4910,7 +5077,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>225</v>
       </c>
@@ -4924,7 +5091,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>226</v>
       </c>
@@ -4938,7 +5105,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>227</v>
       </c>
@@ -4952,7 +5119,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>228</v>
       </c>
@@ -4966,7 +5133,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>229</v>
       </c>
@@ -4980,7 +5147,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>230</v>
       </c>
@@ -4994,7 +5161,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>231</v>
       </c>
@@ -5008,7 +5175,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>232</v>
       </c>
@@ -5022,7 +5189,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>233</v>
       </c>
@@ -5036,7 +5203,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>234</v>
       </c>
@@ -5050,7 +5217,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>235</v>
       </c>
@@ -5064,7 +5231,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>236</v>
       </c>
@@ -5078,7 +5245,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>237</v>
       </c>
@@ -5092,7 +5259,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>238</v>
       </c>
@@ -5106,7 +5273,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>239</v>
       </c>
@@ -5120,7 +5287,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>240</v>
       </c>
@@ -5134,7 +5301,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>241</v>
       </c>
@@ -5148,7 +5315,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>242</v>
       </c>
@@ -5162,7 +5329,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>273</v>
       </c>
@@ -5176,7 +5343,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>274</v>
       </c>
@@ -5190,7 +5357,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>275</v>
       </c>
@@ -5204,7 +5371,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>276</v>
       </c>
@@ -5218,7 +5385,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>277</v>
       </c>
@@ -5232,7 +5399,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>278</v>
       </c>
@@ -5246,7 +5413,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>279</v>
       </c>
@@ -5260,7 +5427,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>280</v>
       </c>
@@ -5274,7 +5441,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>289</v>
       </c>
@@ -5288,7 +5455,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>290</v>
       </c>
@@ -5302,7 +5469,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>291</v>
       </c>
@@ -5316,7 +5483,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>292</v>
       </c>
@@ -5330,7 +5497,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>293</v>
       </c>
@@ -5344,7 +5511,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>294</v>
       </c>
@@ -5358,7 +5525,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>295</v>
       </c>
@@ -5372,7 +5539,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>503</v>
       </c>
@@ -5386,7 +5553,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>504</v>
       </c>
@@ -5400,7 +5567,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>505</v>
       </c>
@@ -5414,7 +5581,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>506</v>
       </c>
@@ -5428,7 +5595,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>507</v>
       </c>
@@ -5442,7 +5609,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>508</v>
       </c>
@@ -5456,7 +5623,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>509</v>
       </c>
@@ -5470,7 +5637,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>510</v>
       </c>
@@ -5484,7 +5651,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>511</v>
       </c>
@@ -5498,7 +5665,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>512</v>
       </c>
@@ -5512,7 +5679,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>513</v>
       </c>
@@ -5526,7 +5693,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>514</v>
       </c>
@@ -5540,7 +5707,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>515</v>
       </c>
@@ -5554,7 +5721,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>516</v>
       </c>
@@ -5568,7 +5735,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>517</v>
       </c>
@@ -5582,7 +5749,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>518</v>
       </c>
@@ -5596,7 +5763,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>519</v>
       </c>
@@ -5610,7 +5777,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>520</v>
       </c>
@@ -5624,7 +5791,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>521</v>
       </c>
@@ -5638,7 +5805,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>522</v>
       </c>
@@ -5652,7 +5819,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>523</v>
       </c>
@@ -5666,7 +5833,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>524</v>
       </c>
@@ -5680,7 +5847,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>525</v>
       </c>
@@ -5694,7 +5861,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>526</v>
       </c>
@@ -5708,7 +5875,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>527</v>
       </c>
@@ -5722,7 +5889,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>528</v>
       </c>
@@ -5736,7 +5903,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>529</v>
       </c>
@@ -5750,7 +5917,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>530</v>
       </c>
@@ -5764,7 +5931,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>531</v>
       </c>
@@ -5778,7 +5945,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>532</v>
       </c>
@@ -5792,7 +5959,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>533</v>
       </c>
@@ -5806,7 +5973,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>534</v>
       </c>
@@ -5820,7 +5987,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>535</v>
       </c>
@@ -5834,7 +6001,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>536</v>
       </c>
@@ -5848,7 +6015,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>537</v>
       </c>
@@ -5862,7 +6029,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>538</v>
       </c>
@@ -5876,7 +6043,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>539</v>
       </c>
@@ -5890,7 +6057,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>540</v>
       </c>
@@ -5904,7 +6071,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>541</v>
       </c>
@@ -5918,7 +6085,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>542</v>
       </c>
@@ -5932,7 +6099,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>305</v>
       </c>
@@ -5946,7 +6113,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>306</v>
       </c>
@@ -5960,7 +6127,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>307</v>
       </c>
@@ -5974,7 +6141,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>308</v>
       </c>
@@ -5988,7 +6155,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>309</v>
       </c>
@@ -6002,7 +6169,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>310</v>
       </c>
@@ -6016,7 +6183,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>311</v>
       </c>
@@ -6033,7 +6200,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>313</v>
       </c>
@@ -6047,7 +6214,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>314</v>
       </c>
@@ -6061,7 +6228,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>315</v>
       </c>
@@ -6075,7 +6242,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>319</v>
       </c>
@@ -6089,7 +6256,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>320</v>
       </c>
@@ -6103,7 +6270,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>321</v>
       </c>
@@ -6117,7 +6284,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>322</v>
       </c>
@@ -6131,7 +6298,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>323</v>
       </c>
@@ -6145,7 +6312,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>324</v>
       </c>
@@ -6159,7 +6326,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>325</v>
       </c>
@@ -6176,7 +6343,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>326</v>
       </c>
@@ -6190,7 +6357,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>327</v>
       </c>
@@ -6204,7 +6371,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>328</v>
       </c>
@@ -6218,7 +6385,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>329</v>
       </c>
@@ -6232,7 +6399,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>330</v>
       </c>
@@ -6246,7 +6413,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>331</v>
       </c>
@@ -6260,7 +6427,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>332</v>
       </c>
@@ -6274,7 +6441,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>333</v>
       </c>
@@ -6288,7 +6455,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>334</v>
       </c>
@@ -6302,7 +6469,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>335</v>
       </c>
@@ -6319,7 +6486,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>336</v>
       </c>
@@ -6333,7 +6500,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>337</v>
       </c>
@@ -6347,7 +6514,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>338</v>
       </c>
@@ -6374,16 +6541,16 @@
       <selection activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -6400,7 +6567,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -6415,7 +6582,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>144</v>
       </c>
@@ -6427,7 +6594,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>145</v>
       </c>
@@ -6439,7 +6606,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>146</v>
       </c>
@@ -6451,7 +6618,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>347</v>
       </c>
@@ -6463,7 +6630,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>346</v>
       </c>
@@ -6475,7 +6642,7 @@
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>147</v>
       </c>
@@ -6487,7 +6654,7 @@
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>497</v>
       </c>
@@ -6499,7 +6666,7 @@
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>498</v>
       </c>
@@ -6511,7 +6678,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>499</v>
       </c>
@@ -6523,7 +6690,7 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>148</v>
       </c>
@@ -6534,7 +6701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>348</v>
       </c>
@@ -6545,7 +6712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>349</v>
       </c>
@@ -6556,7 +6723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>491</v>
       </c>
@@ -6567,7 +6734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>492</v>
       </c>
@@ -6578,7 +6745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>493</v>
       </c>
@@ -6589,7 +6756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>494</v>
       </c>
@@ -6600,7 +6767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>495</v>
       </c>
@@ -6611,7 +6778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>496</v>
       </c>
@@ -6622,7 +6789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>415</v>
       </c>
@@ -6633,7 +6800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>416</v>
       </c>
@@ -6644,7 +6811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>490</v>
       </c>
@@ -6655,7 +6822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>489</v>
       </c>
@@ -6666,7 +6833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>407</v>
       </c>
@@ -6677,7 +6844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>408</v>
       </c>
@@ -6688,7 +6855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>409</v>
       </c>
@@ -6699,7 +6866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>410</v>
       </c>
@@ -6710,7 +6877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>411</v>
       </c>
@@ -6721,7 +6888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>412</v>
       </c>
@@ -6732,7 +6899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>413</v>
       </c>
@@ -6743,7 +6910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>414</v>
       </c>
@@ -6754,7 +6921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>417</v>
       </c>
@@ -6765,7 +6932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>418</v>
       </c>
@@ -6776,7 +6943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>419</v>
       </c>
@@ -6787,7 +6954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>420</v>
       </c>
@@ -6798,7 +6965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>421</v>
       </c>
@@ -6809,7 +6976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>422</v>
       </c>
@@ -6820,7 +6987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>423</v>
       </c>
@@ -6831,7 +6998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>424</v>
       </c>
@@ -6842,7 +7009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>425</v>
       </c>
@@ -6853,7 +7020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>426</v>
       </c>
@@ -6864,7 +7031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>427</v>
       </c>
@@ -6875,7 +7042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>428</v>
       </c>
@@ -6886,7 +7053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>429</v>
       </c>
@@ -6897,7 +7064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>430</v>
       </c>
@@ -6908,7 +7075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>431</v>
       </c>
@@ -6919,7 +7086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>432</v>
       </c>
@@ -6930,7 +7097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>433</v>
       </c>
@@ -6941,7 +7108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>434</v>
       </c>
@@ -6952,7 +7119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>435</v>
       </c>
@@ -6963,7 +7130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>436</v>
       </c>
@@ -6974,7 +7141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>437</v>
       </c>
@@ -6985,7 +7152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>438</v>
       </c>
@@ -6996,7 +7163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>439</v>
       </c>
@@ -7007,7 +7174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>440</v>
       </c>
@@ -7018,7 +7185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>441</v>
       </c>
@@ -7029,7 +7196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>442</v>
       </c>
@@ -7040,7 +7207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>443</v>
       </c>
@@ -7051,7 +7218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>444</v>
       </c>
@@ -7062,7 +7229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>445</v>
       </c>
@@ -7073,7 +7240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>446</v>
       </c>
@@ -7084,7 +7251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>447</v>
       </c>
@@ -7095,7 +7262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>448</v>
       </c>
@@ -7106,7 +7273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>449</v>
       </c>
@@ -7117,7 +7284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>450</v>
       </c>
@@ -7128,7 +7295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>451</v>
       </c>
@@ -7139,7 +7306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>452</v>
       </c>
@@ -7150,7 +7317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>453</v>
       </c>
@@ -7161,7 +7328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>454</v>
       </c>
@@ -7172,7 +7339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>455</v>
       </c>
@@ -7183,7 +7350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>456</v>
       </c>
@@ -7194,7 +7361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>457</v>
       </c>
@@ -7205,7 +7372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>458</v>
       </c>
@@ -7216,7 +7383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>459</v>
       </c>
@@ -7227,7 +7394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>460</v>
       </c>
@@ -7238,7 +7405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>461</v>
       </c>
@@ -7249,7 +7416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>462</v>
       </c>
@@ -7260,7 +7427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>463</v>
       </c>
@@ -7271,7 +7438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>464</v>
       </c>
@@ -7282,7 +7449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>465</v>
       </c>
@@ -7293,7 +7460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>466</v>
       </c>
@@ -7304,7 +7471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>467</v>
       </c>
@@ -7315,7 +7482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>468</v>
       </c>
@@ -7326,7 +7493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>469</v>
       </c>
@@ -7337,7 +7504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>470</v>
       </c>
@@ -7348,7 +7515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>471</v>
       </c>
@@ -7359,7 +7526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>472</v>
       </c>
@@ -7370,7 +7537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>473</v>
       </c>
@@ -7381,7 +7548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>474</v>
       </c>
@@ -7392,7 +7559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>475</v>
       </c>
@@ -7403,7 +7570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>476</v>
       </c>
@@ -7414,7 +7581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>477</v>
       </c>
@@ -7425,7 +7592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>478</v>
       </c>
@@ -7436,7 +7603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>479</v>
       </c>
@@ -7447,7 +7614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>480</v>
       </c>
@@ -7458,7 +7625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>481</v>
       </c>
@@ -7469,7 +7636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>482</v>
       </c>
@@ -7480,7 +7647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>483</v>
       </c>
@@ -7491,7 +7658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>484</v>
       </c>
@@ -7502,7 +7669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>485</v>
       </c>
@@ -7513,7 +7680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>486</v>
       </c>
@@ -7524,7 +7691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>487</v>
       </c>
@@ -7535,7 +7702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>488</v>
       </c>
@@ -7546,7 +7713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>583</v>
       </c>
@@ -7557,7 +7724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>584</v>
       </c>
@@ -7568,7 +7735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>585</v>
       </c>
@@ -7579,7 +7746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>586</v>
       </c>
@@ -7590,7 +7757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>587</v>
       </c>
@@ -7601,7 +7768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>588</v>
       </c>
@@ -7612,7 +7779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>589</v>
       </c>
@@ -7623,7 +7790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>590</v>
       </c>
@@ -7634,7 +7801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>591</v>
       </c>
@@ -7645,7 +7812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>592</v>
       </c>
@@ -7656,7 +7823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>593</v>
       </c>
@@ -7667,7 +7834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>594</v>
       </c>
@@ -7678,7 +7845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>595</v>
       </c>
@@ -7689,7 +7856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>596</v>
       </c>
@@ -7700,7 +7867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>597</v>
       </c>
@@ -7711,7 +7878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>598</v>
       </c>
@@ -7722,7 +7889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>599</v>
       </c>
@@ -7733,7 +7900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>600</v>
       </c>
@@ -7744,7 +7911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
         <v>601</v>
       </c>
@@ -7755,7 +7922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>602</v>
       </c>

</xml_diff>

<commit_message>
Reduce delays to improve UI performance
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\repo\Ellemento\rack_control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\repo\Ellemento_devel\rack_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1970,9 +1970,6 @@
     <t>lastPVvalue</t>
   </si>
   <si>
-    <t>ARRAY [10] OF REAL</t>
-  </si>
-  <si>
     <t>Main state machine current state (for each instance)</t>
   </si>
   <si>
@@ -1991,7 +1988,10 @@
     <t>Store last PV value for comparison whether to run PV change sequence or not</t>
   </si>
   <si>
-    <t>[10(0.0)]</t>
+    <t>ARRAY [10] OF WORD</t>
+  </si>
+  <si>
+    <t>[10(0)]</t>
   </si>
 </sst>
 </file>
@@ -2339,8 +2339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2880,7 +2880,7 @@
         <v>389</v>
       </c>
       <c r="G29" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
@@ -2897,7 +2897,7 @@
         <v>389</v>
       </c>
       <c r="G30" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
@@ -2914,7 +2914,7 @@
         <v>389</v>
       </c>
       <c r="G31" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
@@ -2931,7 +2931,7 @@
         <v>389</v>
       </c>
       <c r="G32" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
@@ -2962,7 +2962,7 @@
         <v>389</v>
       </c>
       <c r="G34" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
@@ -2970,16 +2970,16 @@
         <v>643</v>
       </c>
       <c r="C35">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>644</v>
+        <v>650</v>
       </c>
       <c r="E35" t="s">
         <v>651</v>
       </c>
       <c r="G35" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add pump set point ramp up code.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\repo\Ellemento_devel\rack_control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\repo\Ellemento\rack_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="663">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1992,6 +1992,39 @@
   </si>
   <si>
     <t>[10(0)]</t>
+  </si>
+  <si>
+    <t>pump_rampup_current_state</t>
+  </si>
+  <si>
+    <t>pump_rampup_next_state</t>
+  </si>
+  <si>
+    <t>pump_rampup_current_value</t>
+  </si>
+  <si>
+    <t>lastPumpTargetValue</t>
+  </si>
+  <si>
+    <t>bRunPumpRampup</t>
+  </si>
+  <si>
+    <t>ARRAY [3] OF INT</t>
+  </si>
+  <si>
+    <t>Pump ramp up state machine state</t>
+  </si>
+  <si>
+    <t>Pump ramp up state machine next state</t>
+  </si>
+  <si>
+    <t>Pump ramp up value</t>
+  </si>
+  <si>
+    <t>Pump ramp up previous value</t>
+  </si>
+  <si>
+    <t>Flag for each pump</t>
   </si>
 </sst>
 </file>
@@ -2337,10 +2370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="E25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2980,6 +3013,91 @@
       </c>
       <c r="G35" t="s">
         <v>649</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>652</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>657</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>653</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>657</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>654</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>655</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>656</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement light controller in Shelf UI Fix python script spacing Added PLC2 project (empty)
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="666">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1781,12 +1781,6 @@
     <t>D28420.7</t>
   </si>
   <si>
-    <t>D28421.0</t>
-  </si>
-  <si>
-    <t>D28421.1</t>
-  </si>
-  <si>
     <t>S0_PLC_WORD_ADDR_OFFSET</t>
   </si>
   <si>
@@ -2025,6 +2019,21 @@
   </si>
   <si>
     <t>Flag for each pump</t>
+  </si>
+  <si>
+    <t>D28422.0</t>
+  </si>
+  <si>
+    <t>D28422.1</t>
+  </si>
+  <si>
+    <t>SEC0_LOCK_LIGHT</t>
+  </si>
+  <si>
+    <t>SEC1_LOCK_LIGHT</t>
+  </si>
+  <si>
+    <t>SEC2_LOCK_LIGHT</t>
   </si>
 </sst>
 </file>
@@ -2372,7 +2381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
@@ -2813,7 +2822,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -2825,7 +2834,7 @@
         <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -2864,7 +2873,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2879,12 +2888,12 @@
         <v>133</v>
       </c>
       <c r="G27" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2896,86 +2905,86 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E29" t="s">
         <v>389</v>
       </c>
       <c r="G29" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E30" t="s">
         <v>389</v>
       </c>
       <c r="G30" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E31" t="s">
         <v>389</v>
       </c>
       <c r="G31" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E32" t="s">
         <v>389</v>
       </c>
       <c r="G32" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -2983,7 +2992,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -2995,63 +3004,63 @@
         <v>389</v>
       </c>
       <c r="G34" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C35">
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E35" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="G35" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -3063,12 +3072,12 @@
         <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -3080,12 +3089,12 @@
         <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -3097,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
   </sheetData>
@@ -4379,12 +4388,12 @@
         <v>133</v>
       </c>
       <c r="G4" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -4469,7 +4478,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -4486,7 +4495,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -4503,7 +4512,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -4520,7 +4529,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -4547,8 +4556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6194,7 +6203,7 @@
         <v>541</v>
       </c>
       <c r="B117" t="s">
-        <v>581</v>
+        <v>661</v>
       </c>
       <c r="C117" t="s">
         <v>3</v>
@@ -6208,7 +6217,7 @@
         <v>542</v>
       </c>
       <c r="B118" t="s">
-        <v>582</v>
+        <v>662</v>
       </c>
       <c r="C118" t="s">
         <v>3</v>
@@ -6222,7 +6231,7 @@
         <v>305</v>
       </c>
       <c r="B119" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
@@ -6236,7 +6245,7 @@
         <v>306</v>
       </c>
       <c r="B120" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C120" t="s">
         <v>1</v>
@@ -6250,7 +6259,7 @@
         <v>307</v>
       </c>
       <c r="B121" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C121" t="s">
         <v>1</v>
@@ -6264,7 +6273,7 @@
         <v>308</v>
       </c>
       <c r="B122" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C122" t="s">
         <v>1</v>
@@ -6278,7 +6287,7 @@
         <v>309</v>
       </c>
       <c r="B123" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C123" t="s">
         <v>1</v>
@@ -6292,7 +6301,7 @@
         <v>310</v>
       </c>
       <c r="B124" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C124" t="s">
         <v>1</v>
@@ -6365,7 +6374,7 @@
         <v>319</v>
       </c>
       <c r="B129" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C129" t="s">
         <v>1</v>
@@ -6379,7 +6388,7 @@
         <v>320</v>
       </c>
       <c r="B130" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C130" t="s">
         <v>1</v>
@@ -6393,7 +6402,7 @@
         <v>321</v>
       </c>
       <c r="B131" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C131" t="s">
         <v>1</v>
@@ -6407,7 +6416,7 @@
         <v>322</v>
       </c>
       <c r="B132" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C132" t="s">
         <v>1</v>
@@ -6421,7 +6430,7 @@
         <v>323</v>
       </c>
       <c r="B133" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C133" t="s">
         <v>1</v>
@@ -6435,7 +6444,7 @@
         <v>324</v>
       </c>
       <c r="B134" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C134" t="s">
         <v>1</v>
@@ -6480,7 +6489,7 @@
         <v>327</v>
       </c>
       <c r="B137" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C137" t="s">
         <v>1</v>
@@ -6508,7 +6517,7 @@
         <v>329</v>
       </c>
       <c r="B139" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C139" t="s">
         <v>1</v>
@@ -6522,7 +6531,7 @@
         <v>330</v>
       </c>
       <c r="B140" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C140" t="s">
         <v>1</v>
@@ -6536,7 +6545,7 @@
         <v>331</v>
       </c>
       <c r="B141" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C141" t="s">
         <v>1</v>
@@ -6550,7 +6559,7 @@
         <v>332</v>
       </c>
       <c r="B142" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C142" t="s">
         <v>1</v>
@@ -6564,7 +6573,7 @@
         <v>333</v>
       </c>
       <c r="B143" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C143" t="s">
         <v>1</v>
@@ -6578,7 +6587,7 @@
         <v>334</v>
       </c>
       <c r="B144" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C144" t="s">
         <v>1</v>
@@ -6623,7 +6632,7 @@
         <v>337</v>
       </c>
       <c r="B147" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C147" t="s">
         <v>1</v>
@@ -6653,10 +6662,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6909,21 +6918,21 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>415</v>
+        <v>663</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>416</v>
+        <v>664</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -6931,10 +6940,10 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>490</v>
+        <v>665</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -6942,18 +6951,18 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>489</v>
+        <v>415</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -6964,7 +6973,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>408</v>
+        <v>490</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -6975,7 +6984,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>409</v>
+        <v>489</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -6986,7 +6995,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -6997,7 +7006,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -7008,7 +7017,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -7019,7 +7028,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -7030,7 +7039,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
@@ -7041,7 +7050,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -7052,7 +7061,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -7063,7 +7072,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -7074,7 +7083,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -7085,7 +7094,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -7096,7 +7105,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
@@ -7107,7 +7116,7 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
@@ -7118,7 +7127,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -7129,7 +7138,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
@@ -7140,7 +7149,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -7151,7 +7160,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -7162,7 +7171,7 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
@@ -7173,7 +7182,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
@@ -7184,7 +7193,7 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
@@ -7195,7 +7204,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
@@ -7206,7 +7215,7 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
@@ -7217,7 +7226,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
@@ -7228,7 +7237,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
@@ -7239,7 +7248,7 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
@@ -7250,7 +7259,7 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -7261,7 +7270,7 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
@@ -7272,7 +7281,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
@@ -7283,7 +7292,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
@@ -7294,7 +7303,7 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
@@ -7305,7 +7314,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
@@ -7316,7 +7325,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
@@ -7327,7 +7336,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -7338,7 +7347,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
@@ -7349,7 +7358,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
@@ -7360,7 +7369,7 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
@@ -7371,7 +7380,7 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
@@ -7382,7 +7391,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
@@ -7393,7 +7402,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
@@ -7404,7 +7413,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
@@ -7415,7 +7424,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
@@ -7426,7 +7435,7 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
@@ -7437,7 +7446,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
@@ -7448,7 +7457,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
@@ -7459,7 +7468,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
@@ -7470,7 +7479,7 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
@@ -7481,7 +7490,7 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
@@ -7492,7 +7501,7 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
@@ -7503,7 +7512,7 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
@@ -7514,7 +7523,7 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
@@ -7525,7 +7534,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
@@ -7536,7 +7545,7 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
@@ -7547,7 +7556,7 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
@@ -7558,7 +7567,7 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
@@ -7569,7 +7578,7 @@
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
@@ -7580,7 +7589,7 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
@@ -7591,7 +7600,7 @@
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
@@ -7602,7 +7611,7 @@
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
@@ -7613,7 +7622,7 @@
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
@@ -7624,7 +7633,7 @@
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
@@ -7635,7 +7644,7 @@
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
@@ -7646,7 +7655,7 @@
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
@@ -7657,7 +7666,7 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
@@ -7668,7 +7677,7 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
@@ -7679,7 +7688,7 @@
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
@@ -7690,7 +7699,7 @@
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
@@ -7701,7 +7710,7 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
@@ -7712,7 +7721,7 @@
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
@@ -7723,7 +7732,7 @@
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
@@ -7734,7 +7743,7 @@
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
@@ -7745,7 +7754,7 @@
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
@@ -7756,7 +7765,7 @@
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C98" t="s">
         <v>1</v>
@@ -7767,7 +7776,7 @@
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C99" t="s">
         <v>1</v>
@@ -7778,7 +7787,7 @@
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
@@ -7789,7 +7798,7 @@
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
@@ -7800,7 +7809,7 @@
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
@@ -7811,7 +7820,7 @@
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
@@ -7822,7 +7831,7 @@
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C104" t="s">
         <v>1</v>
@@ -7833,7 +7842,7 @@
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
-        <v>583</v>
+        <v>486</v>
       </c>
       <c r="C105" t="s">
         <v>1</v>
@@ -7844,7 +7853,7 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>584</v>
+        <v>487</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
@@ -7855,7 +7864,7 @@
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
-        <v>585</v>
+        <v>488</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
@@ -7866,7 +7875,7 @@
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
@@ -7877,7 +7886,7 @@
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
@@ -7888,7 +7897,7 @@
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="C110" t="s">
         <v>1</v>
@@ -7899,7 +7908,7 @@
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="C111" t="s">
         <v>1</v>
@@ -7910,7 +7919,7 @@
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="C112" t="s">
         <v>1</v>
@@ -7921,7 +7930,7 @@
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="C113" t="s">
         <v>1</v>
@@ -7932,7 +7941,7 @@
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="C114" t="s">
         <v>1</v>
@@ -7943,7 +7952,7 @@
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="C115" t="s">
         <v>1</v>
@@ -7954,7 +7963,7 @@
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="C116" t="s">
         <v>1</v>
@@ -7965,7 +7974,7 @@
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C117" t="s">
         <v>1</v>
@@ -7976,7 +7985,7 @@
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="C118" t="s">
         <v>1</v>
@@ -7987,7 +7996,7 @@
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
@@ -7998,7 +8007,7 @@
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="C120" t="s">
         <v>1</v>
@@ -8009,7 +8018,7 @@
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="C121" t="s">
         <v>1</v>
@@ -8020,7 +8029,7 @@
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="C122" t="s">
         <v>1</v>
@@ -8031,7 +8040,7 @@
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="C123" t="s">
         <v>1</v>
@@ -8042,12 +8051,45 @@
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="C124" t="s">
         <v>1</v>
       </c>
       <c r="D124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>598</v>
+      </c>
+      <c r="C125" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>599</v>
+      </c>
+      <c r="C126" t="s">
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>600</v>
+      </c>
+      <c r="C127" t="s">
+        <v>1</v>
+      </c>
+      <c r="D127">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix issues with current implementation: - Lighting tested working - Support for multiple shelf working together - Change intensity first before turning ON/OFF LEDs
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\repo\Ellemento\rack_control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\repo\Ellemento_dev\rack_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="713">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2034,6 +2034,147 @@
   </si>
   <si>
     <t>SEC2_LOCK_LIGHT</t>
+  </si>
+  <si>
+    <t>Status for VFD power</t>
+  </si>
+  <si>
+    <t>Status for VFD Comm</t>
+  </si>
+  <si>
+    <t>stat_water_vfd_power1</t>
+  </si>
+  <si>
+    <t>stat_water_vfd_comm1</t>
+  </si>
+  <si>
+    <t>stat_water_vfd_motor1</t>
+  </si>
+  <si>
+    <t>stat_water_vfd_pid1</t>
+  </si>
+  <si>
+    <t>stat_water_vfd_overload1</t>
+  </si>
+  <si>
+    <t>stat_water_shelf_valvefault1</t>
+  </si>
+  <si>
+    <t>stat_water_shelf_overflow1</t>
+  </si>
+  <si>
+    <t>stat_water_temp_range1</t>
+  </si>
+  <si>
+    <t>stat_water_tank_levellow1</t>
+  </si>
+  <si>
+    <t>stat_water_tank_levelhigh1</t>
+  </si>
+  <si>
+    <t>stat_water_tank_sensor_unison1</t>
+  </si>
+  <si>
+    <t>stat_light_powertrip1</t>
+  </si>
+  <si>
+    <t>stat_light_burned1</t>
+  </si>
+  <si>
+    <t>Status for water system</t>
+  </si>
+  <si>
+    <t>Status for lighting system</t>
+  </si>
+  <si>
+    <t>Status for ventilation system</t>
+  </si>
+  <si>
+    <t>stat_vent_vfd_comm1</t>
+  </si>
+  <si>
+    <t>stat_vent_vfd_power1</t>
+  </si>
+  <si>
+    <t>stat_vent_vfd_motor1</t>
+  </si>
+  <si>
+    <t>stat_vent_vfd_overload1</t>
+  </si>
+  <si>
+    <t>stat_vent_air_offline1</t>
+  </si>
+  <si>
+    <t>stat_vent_air_deviation1</t>
+  </si>
+  <si>
+    <t>stat_vent_air_humidity1</t>
+  </si>
+  <si>
+    <t>stat_vent_air_co2</t>
+  </si>
+  <si>
+    <t>stat_vent_air_temp1</t>
+  </si>
+  <si>
+    <t>D200</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>tmpConversionFloat</t>
+  </si>
+  <si>
+    <t>errAnemometer</t>
+  </si>
+  <si>
+    <t>ARRAY[1] OF BOOL</t>
+  </si>
+  <si>
+    <t>[1(FALSE)]</t>
+  </si>
+  <si>
+    <t>Anemometer error (0 = no error)</t>
+  </si>
+  <si>
+    <t>errAQM</t>
+  </si>
+  <si>
+    <t>AQM sensor error (0 = no error)</t>
+  </si>
+  <si>
+    <t>sensorWindSpeed</t>
+  </si>
+  <si>
+    <t>aqmSensorHumidity</t>
+  </si>
+  <si>
+    <t>aqmSensorCO2</t>
+  </si>
+  <si>
+    <t>aqmSensorTemperature</t>
+  </si>
+  <si>
+    <t>tmpCounter</t>
+  </si>
+  <si>
+    <t>ARRAY[1] OF REAL</t>
+  </si>
+  <si>
+    <t>[1(0)]</t>
+  </si>
+  <si>
+    <t>Humdity reading</t>
+  </si>
+  <si>
+    <t>CO2 reading</t>
+  </si>
+  <si>
+    <t>Temperature reading</t>
+  </si>
+  <si>
+    <t>Anemometer reading</t>
   </si>
 </sst>
 </file>
@@ -2379,10 +2520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3109,6 +3250,556 @@
         <v>660</v>
       </c>
     </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>668</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>133</v>
+      </c>
+      <c r="G41" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>669</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>133</v>
+      </c>
+      <c r="G42" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>670</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>133</v>
+      </c>
+      <c r="G43" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>671</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>133</v>
+      </c>
+      <c r="G44" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>672</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>133</v>
+      </c>
+      <c r="G45" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>673</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>133</v>
+      </c>
+      <c r="G46" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>674</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>133</v>
+      </c>
+      <c r="G47" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>675</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>133</v>
+      </c>
+      <c r="G48" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>676</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>133</v>
+      </c>
+      <c r="G49" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>677</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>133</v>
+      </c>
+      <c r="G50" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>678</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>133</v>
+      </c>
+      <c r="G51" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>680</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>133</v>
+      </c>
+      <c r="G52" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>679</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>133</v>
+      </c>
+      <c r="G53" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>684</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>133</v>
+      </c>
+      <c r="G54" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>685</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>133</v>
+      </c>
+      <c r="G55" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>686</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>133</v>
+      </c>
+      <c r="G56" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>687</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>133</v>
+      </c>
+      <c r="G57" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>688</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>133</v>
+      </c>
+      <c r="G58" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>689</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
+        <v>133</v>
+      </c>
+      <c r="G59" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>690</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>133</v>
+      </c>
+      <c r="G60" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>691</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>133</v>
+      </c>
+      <c r="G61" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>692</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
+        <v>133</v>
+      </c>
+      <c r="G62" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>696</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>697</v>
+      </c>
+      <c r="E63" t="s">
+        <v>698</v>
+      </c>
+      <c r="G63" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>700</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>697</v>
+      </c>
+      <c r="E64" t="s">
+        <v>698</v>
+      </c>
+      <c r="G64" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>702</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>707</v>
+      </c>
+      <c r="E65" t="s">
+        <v>708</v>
+      </c>
+      <c r="G65" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>703</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>707</v>
+      </c>
+      <c r="E66" t="s">
+        <v>708</v>
+      </c>
+      <c r="G66" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>704</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>707</v>
+      </c>
+      <c r="E67" t="s">
+        <v>708</v>
+      </c>
+      <c r="G67" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>705</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>707</v>
+      </c>
+      <c r="E68" t="s">
+        <v>708</v>
+      </c>
+      <c r="G68" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>706</v>
+      </c>
+      <c r="D69" t="s">
+        <v>639</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3119,7 +3810,7 @@
   <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4554,10 +5245,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G118" sqref="G118"/>
+    <sheetView topLeftCell="A139" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6655,6 +7346,20 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>695</v>
+      </c>
+      <c r="B149" t="s">
+        <v>693</v>
+      </c>
+      <c r="C149" t="s">
+        <v>694</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6664,7 +7369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A105" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix scheduling system Adjust PV/water system causing the pressure sensor to shoot up. Fix: Open PV first before turning on pump.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -2522,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix global_variable_generator.py to import arrays properly for IO modules Added warning system
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="736">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2181,6 +2181,69 @@
   </si>
   <si>
     <t>Water level</t>
+  </si>
+  <si>
+    <t>Global alarm indicator</t>
+  </si>
+  <si>
+    <t>stat_alarm_clear</t>
+  </si>
+  <si>
+    <t>CONST_AIR_TEMPERATURE_MAX</t>
+  </si>
+  <si>
+    <t>CONST_AIR_TEMPERATURE_MIN</t>
+  </si>
+  <si>
+    <t>CONST_AIR_HUMIDITY_MAX</t>
+  </si>
+  <si>
+    <t>CONST_AIR_HUMIDITY_MIN</t>
+  </si>
+  <si>
+    <t>CONST_AIR_CO2_MAX</t>
+  </si>
+  <si>
+    <t>CONST_AIR_CO2_MIN</t>
+  </si>
+  <si>
+    <t>For range checking</t>
+  </si>
+  <si>
+    <t>MB_pump0_faultRecord</t>
+  </si>
+  <si>
+    <t>D25160</t>
+  </si>
+  <si>
+    <t>[10(-1)]</t>
+  </si>
+  <si>
+    <t>MB_pump1_faultRecord</t>
+  </si>
+  <si>
+    <t>D25360</t>
+  </si>
+  <si>
+    <t>MB_pump2_faultRecord</t>
+  </si>
+  <si>
+    <t>D25560</t>
+  </si>
+  <si>
+    <t>CONST_WATER_RANGE_MAX</t>
+  </si>
+  <si>
+    <t>CONST_WATER_RANGE_MIN</t>
+  </si>
+  <si>
+    <t>Checking water temperature range</t>
+  </si>
+  <si>
+    <t>stat_water_vfd_other1</t>
+  </si>
+  <si>
+    <t>Other VFD error</t>
   </si>
 </sst>
 </file>
@@ -2526,10 +2589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="B39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3358,7 +3421,7 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>673</v>
+        <v>734</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -3373,12 +3436,12 @@
         <v>133</v>
       </c>
       <c r="G46" t="s">
-        <v>681</v>
+        <v>735</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -3398,7 +3461,7 @@
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -3418,7 +3481,7 @@
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -3438,7 +3501,7 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -3458,7 +3521,7 @@
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -3478,7 +3541,7 @@
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -3493,12 +3556,12 @@
         <v>133</v>
       </c>
       <c r="G52" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -3518,7 +3581,7 @@
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3533,12 +3596,12 @@
         <v>133</v>
       </c>
       <c r="G54" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3558,7 +3621,7 @@
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3578,7 +3641,7 @@
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3598,7 +3661,7 @@
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3618,7 +3681,7 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3638,7 +3701,7 @@
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -3658,7 +3721,7 @@
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -3678,7 +3741,7 @@
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -3698,47 +3761,47 @@
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="C63">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>710</v>
-      </c>
-      <c r="E63" t="s">
-        <v>709</v>
+        <v>3</v>
+      </c>
+      <c r="E63" t="b">
+        <v>1</v>
       </c>
       <c r="F63" t="s">
         <v>133</v>
       </c>
       <c r="G63" t="s">
-        <v>697</v>
+        <v>683</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>698</v>
+        <v>716</v>
       </c>
       <c r="C64">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>710</v>
-      </c>
-      <c r="E64" t="s">
-        <v>709</v>
+        <v>3</v>
+      </c>
+      <c r="E64" t="b">
+        <v>1</v>
       </c>
       <c r="F64" t="s">
         <v>133</v>
       </c>
       <c r="G64" t="s">
-        <v>699</v>
+        <v>715</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="C65">
         <v>30</v>
@@ -3753,12 +3816,12 @@
         <v>133</v>
       </c>
       <c r="G65" t="s">
-        <v>708</v>
+        <v>697</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="C66">
         <v>30</v>
@@ -3773,12 +3836,12 @@
         <v>133</v>
       </c>
       <c r="G66" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C67">
         <v>30</v>
@@ -3793,12 +3856,12 @@
         <v>133</v>
       </c>
       <c r="G67" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C68">
         <v>30</v>
@@ -3813,51 +3876,251 @@
         <v>133</v>
       </c>
       <c r="G68" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D69" t="s">
-        <v>639</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
+        <v>710</v>
+      </c>
+      <c r="E69" t="s">
+        <v>709</v>
+      </c>
+      <c r="F69" t="s">
+        <v>133</v>
+      </c>
+      <c r="G69" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D70" t="s">
-        <v>1</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
+        <v>710</v>
+      </c>
+      <c r="E70" t="s">
+        <v>709</v>
+      </c>
+      <c r="F70" t="s">
+        <v>133</v>
       </c>
       <c r="G70" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
+        <v>704</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>639</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>711</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="G72" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>717</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>133</v>
+      </c>
+      <c r="G73" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>718</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>133</v>
+      </c>
+      <c r="G74" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>719</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>133</v>
+      </c>
+      <c r="G75" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>720</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
+        <v>133</v>
+      </c>
+      <c r="G76" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>721</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77" t="s">
+        <v>133</v>
+      </c>
+      <c r="G77" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>722</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78" t="s">
+        <v>133</v>
+      </c>
+      <c r="G78" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>731</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79" t="s">
+        <v>133</v>
+      </c>
+      <c r="G79" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>732</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>133</v>
+      </c>
+      <c r="G80" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
         <v>713</v>
       </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="E71">
+      <c r="E81">
         <v>0</v>
       </c>
     </row>
@@ -5050,7 +5313,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5306,17 +5569,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F149"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="A125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7219,24 +7482,27 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>319</v>
+        <v>724</v>
       </c>
       <c r="B129" t="s">
-        <v>607</v>
-      </c>
-      <c r="C129" t="s">
-        <v>1</v>
-      </c>
-      <c r="D129">
-        <v>-1</v>
+        <v>725</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="D129" t="s">
+        <v>726</v>
+      </c>
+      <c r="E129" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B130" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C130" t="s">
         <v>1</v>
@@ -7247,10 +7513,10 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B131" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C131" t="s">
         <v>1</v>
@@ -7261,10 +7527,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B132" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C132" t="s">
         <v>1</v>
@@ -7275,10 +7541,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B133" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C133" t="s">
         <v>1</v>
@@ -7289,10 +7555,10 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B134" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C134" t="s">
         <v>1</v>
@@ -7303,41 +7569,41 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B135" t="s">
-        <v>339</v>
+        <v>612</v>
       </c>
       <c r="C135" t="s">
         <v>1</v>
       </c>
       <c r="D135">
         <v>-1</v>
-      </c>
-      <c r="E135" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B136" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C136" t="s">
         <v>1</v>
       </c>
       <c r="D136">
         <v>-1</v>
+      </c>
+      <c r="E136" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B137" t="s">
-        <v>613</v>
+        <v>340</v>
       </c>
       <c r="C137" t="s">
         <v>1</v>
@@ -7348,10 +7614,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B138" t="s">
-        <v>341</v>
+        <v>613</v>
       </c>
       <c r="C138" t="s">
         <v>1</v>
@@ -7362,10 +7628,10 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B139" t="s">
-        <v>614</v>
+        <v>341</v>
       </c>
       <c r="C139" t="s">
         <v>1</v>
@@ -7376,24 +7642,27 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>330</v>
+        <v>727</v>
       </c>
       <c r="B140" t="s">
-        <v>615</v>
-      </c>
-      <c r="C140" t="s">
-        <v>1</v>
-      </c>
-      <c r="D140">
-        <v>-1</v>
+        <v>728</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="D140" t="s">
+        <v>726</v>
+      </c>
+      <c r="E140" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B141" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C141" t="s">
         <v>1</v>
@@ -7404,10 +7673,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B142" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C142" t="s">
         <v>1</v>
@@ -7418,10 +7687,10 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B143" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C143" t="s">
         <v>1</v>
@@ -7432,10 +7701,10 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B144" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C144" t="s">
         <v>1</v>
@@ -7446,27 +7715,24 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B145" t="s">
-        <v>342</v>
+        <v>618</v>
       </c>
       <c r="C145" t="s">
         <v>1</v>
       </c>
       <c r="D145">
         <v>-1</v>
-      </c>
-      <c r="E145" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B146" t="s">
-        <v>343</v>
+        <v>619</v>
       </c>
       <c r="C146" t="s">
         <v>1</v>
@@ -7477,24 +7743,27 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B147" t="s">
-        <v>620</v>
+        <v>342</v>
       </c>
       <c r="C147" t="s">
         <v>1</v>
       </c>
       <c r="D147">
         <v>-1</v>
+      </c>
+      <c r="E147" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B148" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C148" t="s">
         <v>1</v>
@@ -7505,15 +7774,60 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>337</v>
+      </c>
+      <c r="B149" t="s">
+        <v>620</v>
+      </c>
+      <c r="C149" t="s">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>338</v>
+      </c>
+      <c r="B150" t="s">
+        <v>344</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>729</v>
+      </c>
+      <c r="B151" t="s">
+        <v>730</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="D151" t="s">
+        <v>726</v>
+      </c>
+      <c r="E151" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>695</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B152" t="s">
         <v>693</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C152" t="s">
         <v>694</v>
       </c>
-      <c r="D149">
+      <c r="D152">
         <v>0</v>
       </c>
     </row>
@@ -7526,7 +7840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Configure airflow vfd Change python script for global variable generator to support new data for PLC2.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -19,6 +19,7 @@
     <sheet name="Pump" sheetId="5" r:id="rId5"/>
     <sheet name="IO Mapping" sheetId="8" r:id="rId6"/>
     <sheet name="HMI Internal" sheetId="7" r:id="rId7"/>
+    <sheet name="PLC2 Global" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="777">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2244,6 +2245,129 @@
   </si>
   <si>
     <t>Other VFD error</t>
+  </si>
+  <si>
+    <t>IO_airflowVfdStartStop</t>
+  </si>
+  <si>
+    <t>IO_airflowVfdFreqCmd</t>
+  </si>
+  <si>
+    <t>IO_airflowVfdInputSrc</t>
+  </si>
+  <si>
+    <t>IO_airflowVfdStatusMonitor</t>
+  </si>
+  <si>
+    <t>D29000</t>
+  </si>
+  <si>
+    <t>D29003</t>
+  </si>
+  <si>
+    <t>D29001</t>
+  </si>
+  <si>
+    <t>D29002</t>
+  </si>
+  <si>
+    <t>ARRAY [23] OF WORD</t>
+  </si>
+  <si>
+    <t>[23(-1)]</t>
+  </si>
+  <si>
+    <t>Airflow VFD in PLC2</t>
+  </si>
+  <si>
+    <t>Status Airflow VFD in PLC2</t>
+  </si>
+  <si>
+    <t>bRunAirflowController</t>
+  </si>
+  <si>
+    <t>Temporary flag to avoid running the code everytime</t>
+  </si>
+  <si>
+    <t>Used for real to word conversion</t>
+  </si>
+  <si>
+    <t>windSpeed</t>
+  </si>
+  <si>
+    <t>airTemp</t>
+  </si>
+  <si>
+    <t>airHumidity</t>
+  </si>
+  <si>
+    <t>airCO2</t>
+  </si>
+  <si>
+    <t>D1000</t>
+  </si>
+  <si>
+    <t>D1200</t>
+  </si>
+  <si>
+    <t>D1400</t>
+  </si>
+  <si>
+    <t>Anemometer reading in cm/s</t>
+  </si>
+  <si>
+    <t>AQM reading</t>
+  </si>
+  <si>
+    <t>Anemometer reading error</t>
+  </si>
+  <si>
+    <t>AQM reading error</t>
+  </si>
+  <si>
+    <t>D1100</t>
+  </si>
+  <si>
+    <t>D1300</t>
+  </si>
+  <si>
+    <t>D1500</t>
+  </si>
+  <si>
+    <t>D26000</t>
+  </si>
+  <si>
+    <t>D26100</t>
+  </si>
+  <si>
+    <t>D26200</t>
+  </si>
+  <si>
+    <t>D26300</t>
+  </si>
+  <si>
+    <t>D26400</t>
+  </si>
+  <si>
+    <t>D26500</t>
+  </si>
+  <si>
+    <t>D205</t>
+  </si>
+  <si>
+    <t>counter for delay</t>
+  </si>
+  <si>
+    <t>airflowVfdSetPoint</t>
+  </si>
+  <si>
+    <t>Airflow target setting</t>
+  </si>
+  <si>
+    <t>airflowVfdOnOff</t>
+  </si>
+  <si>
+    <t>Airflow on/off</t>
   </si>
 </sst>
 </file>
@@ -2254,8 +2378,16 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2289,7 +2421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2308,6 +2440,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2589,10 +2724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3801,158 +3936,158 @@
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>696</v>
+        <v>704</v>
       </c>
       <c r="C65">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>710</v>
-      </c>
-      <c r="E65" t="s">
-        <v>709</v>
-      </c>
-      <c r="F65" t="s">
-        <v>133</v>
-      </c>
-      <c r="G65" t="s">
-        <v>697</v>
+        <v>639</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>698</v>
+        <v>711</v>
       </c>
       <c r="C66">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>710</v>
-      </c>
-      <c r="E66" t="s">
-        <v>709</v>
-      </c>
-      <c r="F66" t="s">
-        <v>133</v>
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>699</v>
+        <v>712</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>700</v>
+        <v>717</v>
       </c>
       <c r="C67">
-        <v>30</v>
-      </c>
-      <c r="D67" t="s">
-        <v>710</v>
-      </c>
-      <c r="E67" t="s">
-        <v>709</v>
+        <v>1</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
       </c>
       <c r="F67" t="s">
         <v>133</v>
       </c>
       <c r="G67" t="s">
-        <v>708</v>
+        <v>723</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>701</v>
+        <v>718</v>
       </c>
       <c r="C68">
-        <v>30</v>
-      </c>
-      <c r="D68" t="s">
-        <v>710</v>
-      </c>
-      <c r="E68" t="s">
-        <v>709</v>
+        <v>1</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
       </c>
       <c r="F68" t="s">
         <v>133</v>
       </c>
       <c r="G68" t="s">
-        <v>705</v>
+        <v>723</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>702</v>
+        <v>719</v>
       </c>
       <c r="C69">
-        <v>30</v>
-      </c>
-      <c r="D69" t="s">
-        <v>710</v>
-      </c>
-      <c r="E69" t="s">
-        <v>709</v>
+        <v>1</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
       </c>
       <c r="F69" t="s">
         <v>133</v>
       </c>
       <c r="G69" t="s">
-        <v>706</v>
+        <v>723</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>703</v>
+        <v>720</v>
       </c>
       <c r="C70">
-        <v>30</v>
-      </c>
-      <c r="D70" t="s">
-        <v>710</v>
-      </c>
-      <c r="E70" t="s">
-        <v>709</v>
+        <v>1</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
       </c>
       <c r="F70" t="s">
         <v>133</v>
       </c>
       <c r="G70" t="s">
-        <v>707</v>
+        <v>723</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>704</v>
+        <v>721</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
-      <c r="D71" t="s">
-        <v>639</v>
+      <c r="D71" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
+      <c r="F71" t="s">
+        <v>133</v>
+      </c>
+      <c r="G71" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>711</v>
+        <v>722</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="8" t="s">
         <v>1</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
+      <c r="F72" t="s">
+        <v>133</v>
+      </c>
       <c r="G72" t="s">
-        <v>712</v>
+        <v>723</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>717</v>
+        <v>731</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -3967,12 +4102,12 @@
         <v>133</v>
       </c>
       <c r="G73" t="s">
-        <v>723</v>
+        <v>733</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>718</v>
+        <v>732</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -3987,32 +4122,29 @@
         <v>133</v>
       </c>
       <c r="G74" t="s">
-        <v>723</v>
+        <v>733</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>719</v>
+        <v>748</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75" t="s">
-        <v>133</v>
+        <v>3</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>723</v>
+        <v>749</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>720</v>
+        <v>773</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4021,106 +4153,46 @@
         <v>1</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="F76" t="s">
         <v>133</v>
       </c>
       <c r="G76" t="s">
-        <v>723</v>
+        <v>774</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>721</v>
+        <v>775</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E77" t="b">
+        <v>1</v>
       </c>
       <c r="F77" t="s">
         <v>133</v>
       </c>
       <c r="G77" t="s">
-        <v>723</v>
+        <v>776</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>1</v>
+        <v>694</v>
       </c>
       <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78" t="s">
-        <v>133</v>
-      </c>
-      <c r="G78" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
-        <v>731</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79" t="s">
-        <v>133</v>
-      </c>
-      <c r="G79" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
-        <v>732</v>
-      </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80" t="s">
-        <v>133</v>
-      </c>
-      <c r="G80" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B81" t="s">
-        <v>713</v>
-      </c>
-      <c r="C81">
-        <v>2</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="E81">
         <v>0</v>
       </c>
     </row>
@@ -5569,10 +5641,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+    <sheetView topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5581,6 +5653,7 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.109375" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -7713,7 +7786,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>333</v>
       </c>
@@ -7727,7 +7800,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>334</v>
       </c>
@@ -7741,7 +7814,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>335</v>
       </c>
@@ -7758,7 +7831,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>336</v>
       </c>
@@ -7772,7 +7845,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>337</v>
       </c>
@@ -7786,7 +7859,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>338</v>
       </c>
@@ -7800,7 +7873,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>729</v>
       </c>
@@ -7817,18 +7890,206 @@
         <v>133</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
+        <v>736</v>
+      </c>
+      <c r="B152" t="s">
+        <v>740</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1</v>
+      </c>
+      <c r="D152">
+        <v>-1</v>
+      </c>
+      <c r="F152" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>737</v>
+      </c>
+      <c r="B153" t="s">
+        <v>742</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>-1</v>
+      </c>
+      <c r="F153" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>738</v>
+      </c>
+      <c r="B154" t="s">
+        <v>743</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1</v>
+      </c>
+      <c r="D154">
+        <v>-1</v>
+      </c>
+      <c r="F154" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>739</v>
+      </c>
+      <c r="B155" t="s">
+        <v>741</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="D155" t="s">
+        <v>745</v>
+      </c>
+      <c r="F155" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>695</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B156" t="s">
         <v>693</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C156" t="s">
         <v>694</v>
       </c>
-      <c r="D152">
+      <c r="D156">
         <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>700</v>
+      </c>
+      <c r="B157" t="s">
+        <v>765</v>
+      </c>
+      <c r="C157" t="s">
+        <v>710</v>
+      </c>
+      <c r="D157" t="s">
+        <v>709</v>
+      </c>
+      <c r="E157" t="s">
+        <v>133</v>
+      </c>
+      <c r="F157" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>703</v>
+      </c>
+      <c r="B158" t="s">
+        <v>766</v>
+      </c>
+      <c r="C158" t="s">
+        <v>710</v>
+      </c>
+      <c r="D158" t="s">
+        <v>709</v>
+      </c>
+      <c r="E158" t="s">
+        <v>133</v>
+      </c>
+      <c r="F158" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>701</v>
+      </c>
+      <c r="B159" t="s">
+        <v>767</v>
+      </c>
+      <c r="C159" t="s">
+        <v>710</v>
+      </c>
+      <c r="D159" t="s">
+        <v>709</v>
+      </c>
+      <c r="E159" t="s">
+        <v>133</v>
+      </c>
+      <c r="F159" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>702</v>
+      </c>
+      <c r="B160" t="s">
+        <v>768</v>
+      </c>
+      <c r="C160" t="s">
+        <v>710</v>
+      </c>
+      <c r="D160" t="s">
+        <v>709</v>
+      </c>
+      <c r="E160" t="s">
+        <v>133</v>
+      </c>
+      <c r="F160" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>696</v>
+      </c>
+      <c r="B161" t="s">
+        <v>769</v>
+      </c>
+      <c r="C161" t="s">
+        <v>710</v>
+      </c>
+      <c r="D161" t="s">
+        <v>709</v>
+      </c>
+      <c r="E161" t="s">
+        <v>133</v>
+      </c>
+      <c r="F161" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>698</v>
+      </c>
+      <c r="B162" t="s">
+        <v>770</v>
+      </c>
+      <c r="C162" t="s">
+        <v>710</v>
+      </c>
+      <c r="D162" t="s">
+        <v>709</v>
+      </c>
+      <c r="E162" t="s">
+        <v>133</v>
+      </c>
+      <c r="F162" t="s">
+        <v>699</v>
       </c>
     </row>
   </sheetData>
@@ -9272,4 +9533,178 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>695</v>
+      </c>
+      <c r="B2" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2" t="s">
+        <v>694</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>704</v>
+      </c>
+      <c r="B3" t="s">
+        <v>771</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>751</v>
+      </c>
+      <c r="B4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="E4" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>752</v>
+      </c>
+      <c r="B5" t="s">
+        <v>762</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="E5" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>753</v>
+      </c>
+      <c r="B6" t="s">
+        <v>756</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="E6" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>754</v>
+      </c>
+      <c r="B7" t="s">
+        <v>763</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="E7" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>696</v>
+      </c>
+      <c r="B8" t="s">
+        <v>757</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="E8" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>698</v>
+      </c>
+      <c r="B9" t="s">
+        <v>764</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="E9" t="s">
+        <v>761</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Move PLC1 code for air flow sensors to PLC2.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="785">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2368,6 +2368,30 @@
   </si>
   <si>
     <t>Airflow on/off</t>
+  </si>
+  <si>
+    <t>deviceReadState</t>
+  </si>
+  <si>
+    <t>D2000</t>
+  </si>
+  <si>
+    <t>deviceIndex</t>
+  </si>
+  <si>
+    <t>D2001</t>
+  </si>
+  <si>
+    <t>D2002</t>
+  </si>
+  <si>
+    <t>CONST_NUM_ANEMOMETER</t>
+  </si>
+  <si>
+    <t>CONST_NUM_AQM_SENSOR</t>
+  </si>
+  <si>
+    <t>D2003</t>
   </si>
 </sst>
 </file>
@@ -2726,7 +2750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
@@ -9537,15 +9561,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
@@ -9703,6 +9727,62 @@
         <v>761</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>777</v>
+      </c>
+      <c r="B10" t="s">
+        <v>778</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>779</v>
+      </c>
+      <c r="B11" t="s">
+        <v>780</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>782</v>
+      </c>
+      <c r="B12" t="s">
+        <v>781</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>783</v>
+      </c>
+      <c r="B13" t="s">
+        <v>784</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix bug in HMI: wrong variable assignment Experiment with modbus sensors, partially working. Only need to fix the 2nd sensor issue.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="792">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2376,9 +2376,6 @@
     <t>D2000</t>
   </si>
   <si>
-    <t>deviceIndex</t>
-  </si>
-  <si>
     <t>D2001</t>
   </si>
   <si>
@@ -2392,6 +2389,30 @@
   </si>
   <si>
     <t>D2003</t>
+  </si>
+  <si>
+    <t>gDeviceIndex</t>
+  </si>
+  <si>
+    <t>gDevice2Index</t>
+  </si>
+  <si>
+    <t>D2004</t>
+  </si>
+  <si>
+    <t>errorVFD</t>
+  </si>
+  <si>
+    <t>D3000</t>
+  </si>
+  <si>
+    <t>Transfer VFD error flag to PLC1</t>
+  </si>
+  <si>
+    <t>errorAirVFD</t>
+  </si>
+  <si>
+    <t>D27000</t>
   </si>
 </sst>
 </file>
@@ -5665,10 +5686,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F162"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
     <sheetView topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F159" sqref="F159"/>
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8114,6 +8135,20 @@
       </c>
       <c r="F162" t="s">
         <v>699</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>790</v>
+      </c>
+      <c r="B163" t="s">
+        <v>791</v>
+      </c>
+      <c r="C163" t="s">
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9561,10 +9596,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9743,10 +9778,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>784</v>
+      </c>
+      <c r="B11" t="s">
         <v>779</v>
-      </c>
-      <c r="B11" t="s">
-        <v>780</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>639</v>
@@ -9757,10 +9792,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="B12" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>639</v>
@@ -9771,16 +9806,47 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>781</v>
+      </c>
+      <c r="B13" t="s">
         <v>783</v>
-      </c>
-      <c r="B13" t="s">
-        <v>784</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>639</v>
       </c>
       <c r="D13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>782</v>
+      </c>
+      <c r="B14" t="s">
+        <v>786</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>787</v>
+      </c>
+      <c r="B15" t="s">
+        <v>788</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extend Log file length Reduce attempts of reading sensors.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="800">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2413,6 +2413,30 @@
   </si>
   <si>
     <t>D27000</t>
+  </si>
+  <si>
+    <t>stat_plc1_system</t>
+  </si>
+  <si>
+    <t>stat_plc2_system</t>
+  </si>
+  <si>
+    <t>PLC1 system</t>
+  </si>
+  <si>
+    <t>PLC2 system</t>
+  </si>
+  <si>
+    <t>stat_plc1_io</t>
+  </si>
+  <si>
+    <t>PLC1 IO</t>
+  </si>
+  <si>
+    <t>stat_plc2_io</t>
+  </si>
+  <si>
+    <t>PLC2 IO</t>
   </si>
 </sst>
 </file>
@@ -2769,10 +2793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3981,118 +4005,118 @@
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>704</v>
+        <v>792</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>639</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>133</v>
+      </c>
+      <c r="G65" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>711</v>
+        <v>793</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>1</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>133</v>
       </c>
       <c r="G66" t="s">
-        <v>712</v>
+        <v>795</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>717</v>
+        <v>796</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
-      <c r="D67" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
+      <c r="D67" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" t="b">
+        <v>1</v>
       </c>
       <c r="F67" t="s">
         <v>133</v>
       </c>
       <c r="G67" t="s">
-        <v>723</v>
+        <v>797</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>718</v>
+        <v>798</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
-      <c r="D68" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
+      <c r="D68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" t="b">
+        <v>1</v>
       </c>
       <c r="F68" t="s">
         <v>133</v>
       </c>
       <c r="G68" t="s">
-        <v>723</v>
+        <v>799</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>719</v>
+        <v>704</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
-      <c r="D69" s="8" t="s">
-        <v>1</v>
+      <c r="D69" t="s">
+        <v>639</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
-      <c r="F69" t="s">
-        <v>133</v>
-      </c>
-      <c r="G69" t="s">
-        <v>723</v>
-      </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" t="s">
         <v>1</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
-      <c r="F70" t="s">
-        <v>133</v>
-      </c>
       <c r="G70" t="s">
-        <v>723</v>
+        <v>712</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -4112,7 +4136,7 @@
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4132,7 +4156,7 @@
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>731</v>
+        <v>719</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4147,12 +4171,12 @@
         <v>133</v>
       </c>
       <c r="G73" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>732</v>
+        <v>720</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4167,29 +4191,32 @@
         <v>133</v>
       </c>
       <c r="G74" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>748</v>
+        <v>721</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E75" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>133</v>
       </c>
       <c r="G75" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>773</v>
+        <v>722</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4198,46 +4225,123 @@
         <v>1</v>
       </c>
       <c r="E76">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="F76" t="s">
         <v>133</v>
       </c>
       <c r="G76" t="s">
-        <v>774</v>
+        <v>723</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>775</v>
+        <v>731</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E77" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
       </c>
       <c r="F77" t="s">
         <v>133</v>
       </c>
       <c r="G77" t="s">
-        <v>776</v>
+        <v>733</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
+        <v>732</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78" t="s">
+        <v>133</v>
+      </c>
+      <c r="G78" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>748</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
+      <c r="G79" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>773</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>3000</v>
+      </c>
+      <c r="F80" t="s">
+        <v>133</v>
+      </c>
+      <c r="G80" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>775</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" t="s">
+        <v>133</v>
+      </c>
+      <c r="G81" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
         <v>713</v>
       </c>
-      <c r="C78">
+      <c r="C82">
         <v>2</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D82" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="E78">
+      <c r="E82">
         <v>0</v>
       </c>
     </row>
@@ -5688,7 +5792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
@@ -9598,7 +9702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix AQM sensor reading in HMI. Added new check for PLC2. Added transfer warning.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="815">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2437,6 +2437,51 @@
   </si>
   <si>
     <t>PLC2 IO</t>
+  </si>
+  <si>
+    <t>errorSystem</t>
+  </si>
+  <si>
+    <t>D3001</t>
+  </si>
+  <si>
+    <t>errorIO</t>
+  </si>
+  <si>
+    <t>D3002</t>
+  </si>
+  <si>
+    <t>Transfer PLC system error to PLC1</t>
+  </si>
+  <si>
+    <t>Transfer PLC I/O error to PLC1</t>
+  </si>
+  <si>
+    <t>errorPLC2system</t>
+  </si>
+  <si>
+    <t>errorPLC2io</t>
+  </si>
+  <si>
+    <t>D27001</t>
+  </si>
+  <si>
+    <t>D27002</t>
+  </si>
+  <si>
+    <t>PLC2 VFD error</t>
+  </si>
+  <si>
+    <t>PLC2 system error</t>
+  </si>
+  <si>
+    <t>PLC2 IO error</t>
+  </si>
+  <si>
+    <t>stat_plc_transfer</t>
+  </si>
+  <si>
+    <t>Transfer between PLC1 and PLC2</t>
   </si>
 </sst>
 </file>
@@ -2793,10 +2838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4085,58 +4130,58 @@
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>704</v>
+        <v>813</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>639</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>133</v>
+      </c>
+      <c r="G69" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>1</v>
+        <v>639</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
-      <c r="G70" t="s">
-        <v>712</v>
-      </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" t="s">
         <v>1</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
-      <c r="F71" t="s">
-        <v>133</v>
-      </c>
       <c r="G71" t="s">
-        <v>723</v>
+        <v>712</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4156,7 +4201,7 @@
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4176,7 +4221,7 @@
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4196,7 +4241,7 @@
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -4216,7 +4261,7 @@
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4236,7 +4281,7 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -4251,12 +4296,12 @@
         <v>133</v>
       </c>
       <c r="G77" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -4276,72 +4321,92 @@
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>748</v>
+        <v>732</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E79" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79" t="s">
+        <v>133</v>
       </c>
       <c r="G79" t="s">
-        <v>749</v>
+        <v>733</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>773</v>
+        <v>748</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E80">
-        <v>3000</v>
-      </c>
-      <c r="F80" t="s">
-        <v>133</v>
+        <v>3</v>
+      </c>
+      <c r="E80" t="b">
+        <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>774</v>
+        <v>749</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E81" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>3000</v>
       </c>
       <c r="F81" t="s">
         <v>133</v>
       </c>
       <c r="G81" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
+        <v>775</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
+        <v>133</v>
+      </c>
+      <c r="G82" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
         <v>713</v>
       </c>
-      <c r="C82">
+      <c r="C83">
         <v>2</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D83" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="E82">
+      <c r="E83">
         <v>0</v>
       </c>
     </row>
@@ -5790,10 +5855,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F163"/>
+  <dimension ref="A1:F165"/>
   <sheetViews>
     <sheetView topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+      <selection activeCell="H163" sqref="H163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8253,6 +8318,43 @@
       </c>
       <c r="D163">
         <v>0</v>
+      </c>
+      <c r="F163" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>806</v>
+      </c>
+      <c r="B164" t="s">
+        <v>808</v>
+      </c>
+      <c r="C164" t="s">
+        <v>1</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="F164" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>807</v>
+      </c>
+      <c r="B165" t="s">
+        <v>809</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1</v>
+      </c>
+      <c r="D165">
+        <v>0</v>
+      </c>
+      <c r="F165" t="s">
+        <v>812</v>
       </c>
     </row>
   </sheetData>
@@ -9700,10 +9802,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9953,6 +10055,40 @@
         <v>789</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>800</v>
+      </c>
+      <c r="B16" t="s">
+        <v>801</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>802</v>
+      </c>
+      <c r="B17" t="s">
+        <v>803</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>805</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Enabled the various ventilation sensors.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="818">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2482,6 +2482,15 @@
   </si>
   <si>
     <t>Transfer between PLC1 and PLC2</t>
+  </si>
+  <si>
+    <t>Ventilation VFD status code</t>
+  </si>
+  <si>
+    <t>stat_vent_vfd_status_code</t>
+  </si>
+  <si>
+    <t>VENTILATION_VFD_STATUS_CODE</t>
   </si>
 </sst>
 </file>
@@ -2838,10 +2847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3930,27 +3939,27 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>688</v>
+        <v>816</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>3</v>
-      </c>
-      <c r="E59" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
       </c>
       <c r="F59" t="s">
         <v>133</v>
       </c>
       <c r="G59" t="s">
-        <v>683</v>
+        <v>815</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -3970,7 +3979,7 @@
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -3990,7 +3999,7 @@
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -4010,7 +4019,7 @@
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -4030,7 +4039,7 @@
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>716</v>
+        <v>692</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -4045,12 +4054,12 @@
         <v>133</v>
       </c>
       <c r="G64" t="s">
-        <v>715</v>
+        <v>683</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>792</v>
+        <v>716</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -4065,12 +4074,12 @@
         <v>133</v>
       </c>
       <c r="G65" t="s">
-        <v>794</v>
+        <v>715</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -4085,12 +4094,12 @@
         <v>133</v>
       </c>
       <c r="G66" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -4105,12 +4114,12 @@
         <v>133</v>
       </c>
       <c r="G67" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -4125,12 +4134,12 @@
         <v>133</v>
       </c>
       <c r="G68" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>813</v>
+        <v>798</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -4145,63 +4154,63 @@
         <v>133</v>
       </c>
       <c r="G69" t="s">
-        <v>814</v>
+        <v>799</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>704</v>
+        <v>813</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>639</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>133</v>
+      </c>
+      <c r="G70" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>1</v>
+        <v>639</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
-      <c r="G71" t="s">
-        <v>712</v>
-      </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="D72" t="s">
         <v>1</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
-      <c r="F72" t="s">
-        <v>133</v>
-      </c>
       <c r="G72" t="s">
-        <v>723</v>
+        <v>712</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4221,7 +4230,7 @@
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4241,7 +4250,7 @@
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -4261,7 +4270,7 @@
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4281,7 +4290,7 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -4301,7 +4310,7 @@
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -4316,12 +4325,12 @@
         <v>133</v>
       </c>
       <c r="G78" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -4341,72 +4350,92 @@
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>748</v>
+        <v>732</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E80" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>133</v>
       </c>
       <c r="G80" t="s">
-        <v>749</v>
+        <v>733</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>773</v>
+        <v>748</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E81">
-        <v>3000</v>
-      </c>
-      <c r="F81" t="s">
-        <v>133</v>
+        <v>3</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>774</v>
+        <v>749</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E82" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>3000</v>
       </c>
       <c r="F82" t="s">
         <v>133</v>
       </c>
       <c r="G82" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
+        <v>775</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E83" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
+        <v>133</v>
+      </c>
+      <c r="G83" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
         <v>713</v>
       </c>
-      <c r="C83">
+      <c r="C84">
         <v>2</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D84" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="E83">
+      <c r="E84">
         <v>0</v>
       </c>
     </row>
@@ -8364,10 +8393,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G127"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9792,6 +9821,17 @@
         <v>1</v>
       </c>
       <c r="D127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>817</v>
+      </c>
+      <c r="C128" t="s">
+        <v>143</v>
+      </c>
+      <c r="D128">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix pump VFD status addresses (bug) Added check for PID warning (60Hz) Added PLC value and ventilation VFD status code in log file
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="828">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1878,9 +1878,6 @@
     <t>D25355</t>
   </si>
   <si>
-    <t>D25301</t>
-  </si>
-  <si>
     <t>D25550</t>
   </si>
   <si>
@@ -1899,9 +1896,6 @@
     <t>D25555</t>
   </si>
   <si>
-    <t>D25501</t>
-  </si>
-  <si>
     <t>flowrate per shelf in lpm</t>
   </si>
   <si>
@@ -2490,7 +2484,43 @@
     <t>stat_vent_vfd_status_code</t>
   </si>
   <si>
-    <t>VENTILATION_VFD_STATUS_CODE</t>
+    <t>D25201</t>
+  </si>
+  <si>
+    <t>D25401</t>
+  </si>
+  <si>
+    <t>Start stop</t>
+  </si>
+  <si>
+    <t>Frequency command</t>
+  </si>
+  <si>
+    <t>Freq command source</t>
+  </si>
+  <si>
+    <t>Terminal session for PID feedback</t>
+  </si>
+  <si>
+    <t>PID target source</t>
+  </si>
+  <si>
+    <t>PID target value</t>
+  </si>
+  <si>
+    <t>Actual output freq</t>
+  </si>
+  <si>
+    <t>ACI val</t>
+  </si>
+  <si>
+    <t>VFD status</t>
+  </si>
+  <si>
+    <t>History of faults</t>
+  </si>
+  <si>
+    <t>VENTILATION_VFD_STATUS_FLAG</t>
   </si>
 </sst>
 </file>
@@ -3290,7 +3320,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -3302,7 +3332,7 @@
         <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -3341,7 +3371,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3356,12 +3386,12 @@
         <v>133</v>
       </c>
       <c r="G27" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3373,86 +3403,86 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E29" t="s">
         <v>389</v>
       </c>
       <c r="G29" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E30" t="s">
         <v>389</v>
       </c>
       <c r="G30" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E31" t="s">
         <v>389</v>
       </c>
       <c r="G31" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E32" t="s">
         <v>389</v>
       </c>
       <c r="G32" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -3460,7 +3490,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -3472,63 +3502,63 @@
         <v>389</v>
       </c>
       <c r="G34" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C35">
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E35" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="G35" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -3540,12 +3570,12 @@
         <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -3557,12 +3587,12 @@
         <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -3574,12 +3604,12 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -3594,12 +3624,12 @@
         <v>133</v>
       </c>
       <c r="G41" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -3614,12 +3644,12 @@
         <v>133</v>
       </c>
       <c r="G42" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3634,12 +3664,12 @@
         <v>133</v>
       </c>
       <c r="G43" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -3654,12 +3684,12 @@
         <v>133</v>
       </c>
       <c r="G44" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3674,12 +3704,12 @@
         <v>133</v>
       </c>
       <c r="G45" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -3694,12 +3724,12 @@
         <v>133</v>
       </c>
       <c r="G46" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -3714,12 +3744,12 @@
         <v>133</v>
       </c>
       <c r="G47" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -3734,12 +3764,12 @@
         <v>133</v>
       </c>
       <c r="G48" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -3754,12 +3784,12 @@
         <v>133</v>
       </c>
       <c r="G49" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -3774,12 +3804,12 @@
         <v>133</v>
       </c>
       <c r="G50" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -3794,12 +3824,12 @@
         <v>133</v>
       </c>
       <c r="G51" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -3814,12 +3844,12 @@
         <v>133</v>
       </c>
       <c r="G52" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -3834,12 +3864,12 @@
         <v>133</v>
       </c>
       <c r="G53" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3854,12 +3884,12 @@
         <v>133</v>
       </c>
       <c r="G54" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3874,12 +3904,12 @@
         <v>133</v>
       </c>
       <c r="G55" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3894,12 +3924,12 @@
         <v>133</v>
       </c>
       <c r="G56" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3914,12 +3944,12 @@
         <v>133</v>
       </c>
       <c r="G57" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3934,12 +3964,12 @@
         <v>133</v>
       </c>
       <c r="G58" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3954,12 +3984,12 @@
         <v>133</v>
       </c>
       <c r="G59" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -3974,12 +4004,12 @@
         <v>133</v>
       </c>
       <c r="G60" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -3994,12 +4024,12 @@
         <v>133</v>
       </c>
       <c r="G61" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -4014,12 +4044,12 @@
         <v>133</v>
       </c>
       <c r="G62" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -4034,12 +4064,12 @@
         <v>133</v>
       </c>
       <c r="G63" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -4054,12 +4084,12 @@
         <v>133</v>
       </c>
       <c r="G64" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -4074,12 +4104,12 @@
         <v>133</v>
       </c>
       <c r="G65" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -4094,12 +4124,12 @@
         <v>133</v>
       </c>
       <c r="G66" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -4114,12 +4144,12 @@
         <v>133</v>
       </c>
       <c r="G67" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -4134,12 +4164,12 @@
         <v>133</v>
       </c>
       <c r="G68" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -4154,12 +4184,12 @@
         <v>133</v>
       </c>
       <c r="G69" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -4174,18 +4204,18 @@
         <v>133</v>
       </c>
       <c r="G70" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -4193,7 +4223,7 @@
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4205,12 +4235,12 @@
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4225,12 +4255,12 @@
         <v>133</v>
       </c>
       <c r="G73" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4245,12 +4275,12 @@
         <v>133</v>
       </c>
       <c r="G74" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -4265,12 +4295,12 @@
         <v>133</v>
       </c>
       <c r="G75" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4285,12 +4315,12 @@
         <v>133</v>
       </c>
       <c r="G76" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -4305,12 +4335,12 @@
         <v>133</v>
       </c>
       <c r="G77" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -4325,12 +4355,12 @@
         <v>133</v>
       </c>
       <c r="G78" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -4345,12 +4375,12 @@
         <v>133</v>
       </c>
       <c r="G79" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -4365,12 +4395,12 @@
         <v>133</v>
       </c>
       <c r="G80" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -4382,12 +4412,12 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4402,12 +4432,12 @@
         <v>133</v>
       </c>
       <c r="G82" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -4422,18 +4452,18 @@
         <v>133</v>
       </c>
       <c r="G83" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C84">
         <v>2</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -5718,12 +5748,12 @@
         <v>133</v>
       </c>
       <c r="G4" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -5808,7 +5838,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -5825,7 +5855,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -5842,7 +5872,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -5859,7 +5889,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -5886,8 +5916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H163" sqref="H163"/>
+    <sheetView topLeftCell="A135" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H144" sqref="H144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6804,7 +6834,7 @@
         <v>133</v>
       </c>
       <c r="F64" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -6824,7 +6854,7 @@
         <v>133</v>
       </c>
       <c r="F65" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -6844,7 +6874,7 @@
         <v>133</v>
       </c>
       <c r="F66" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -6864,7 +6894,7 @@
         <v>133</v>
       </c>
       <c r="F67" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -6884,7 +6914,7 @@
         <v>133</v>
       </c>
       <c r="F68" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -6904,7 +6934,7 @@
         <v>133</v>
       </c>
       <c r="F69" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -7569,7 +7599,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>537</v>
       </c>
@@ -7583,7 +7613,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>538</v>
       </c>
@@ -7597,7 +7627,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>539</v>
       </c>
@@ -7611,7 +7641,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>540</v>
       </c>
@@ -7625,12 +7655,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>541</v>
       </c>
       <c r="B117" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C117" t="s">
         <v>3</v>
@@ -7639,12 +7669,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>542</v>
       </c>
       <c r="B118" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C118" t="s">
         <v>3</v>
@@ -7653,7 +7683,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>305</v>
       </c>
@@ -7666,8 +7696,11 @@
       <c r="D119">
         <v>-1</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F119" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>306</v>
       </c>
@@ -7680,8 +7713,11 @@
       <c r="D120">
         <v>-1</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F120" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>307</v>
       </c>
@@ -7694,8 +7730,11 @@
       <c r="D121">
         <v>-1</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F121" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>308</v>
       </c>
@@ -7708,8 +7747,11 @@
       <c r="D122">
         <v>-1</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F122" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>309</v>
       </c>
@@ -7722,8 +7764,11 @@
       <c r="D123">
         <v>-1</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F123" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>310</v>
       </c>
@@ -7736,8 +7781,11 @@
       <c r="D124">
         <v>-1</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F124" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>311</v>
       </c>
@@ -7753,8 +7801,11 @@
       <c r="E125" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F125" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>313</v>
       </c>
@@ -7767,8 +7818,11 @@
       <c r="D126">
         <v>-1</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F126" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>314</v>
       </c>
@@ -7781,8 +7835,11 @@
       <c r="D127">
         <v>-1</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F127" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>315</v>
       </c>
@@ -7796,24 +7853,27 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
+        <v>722</v>
+      </c>
+      <c r="B129" t="s">
+        <v>723</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="D129" t="s">
         <v>724</v>
       </c>
-      <c r="B129" t="s">
-        <v>725</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D129" t="s">
-        <v>726</v>
-      </c>
       <c r="E129" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F129" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>319</v>
       </c>
@@ -7826,8 +7886,11 @@
       <c r="D130">
         <v>-1</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F130" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>320</v>
       </c>
@@ -7840,8 +7903,11 @@
       <c r="D131">
         <v>-1</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F131" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>321</v>
       </c>
@@ -7854,8 +7920,11 @@
       <c r="D132">
         <v>-1</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F132" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>322</v>
       </c>
@@ -7868,8 +7937,11 @@
       <c r="D133">
         <v>-1</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F133" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>323</v>
       </c>
@@ -7882,8 +7954,11 @@
       <c r="D134">
         <v>-1</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F134" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>324</v>
       </c>
@@ -7896,8 +7971,11 @@
       <c r="D135">
         <v>-1</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F135" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>325</v>
       </c>
@@ -7913,8 +7991,11 @@
       <c r="E136" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F136" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>326</v>
       </c>
@@ -7927,13 +8008,16 @@
       <c r="D137">
         <v>-1</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F137" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>327</v>
       </c>
       <c r="B138" t="s">
-        <v>613</v>
+        <v>815</v>
       </c>
       <c r="C138" t="s">
         <v>1</v>
@@ -7941,8 +8025,11 @@
       <c r="D138">
         <v>-1</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F138" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>328</v>
       </c>
@@ -7956,29 +8043,32 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B140" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D140" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="E140" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F140" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>329</v>
       </c>
       <c r="B141" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C141" t="s">
         <v>1</v>
@@ -7986,13 +8076,16 @@
       <c r="D141">
         <v>-1</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F141" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>330</v>
       </c>
       <c r="B142" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C142" t="s">
         <v>1</v>
@@ -8000,13 +8093,16 @@
       <c r="D142">
         <v>-1</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F142" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>331</v>
       </c>
       <c r="B143" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C143" t="s">
         <v>1</v>
@@ -8014,19 +8110,25 @@
       <c r="D143">
         <v>-1</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F143" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>332</v>
       </c>
       <c r="B144" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C144" t="s">
         <v>1</v>
       </c>
       <c r="D144">
         <v>-1</v>
+      </c>
+      <c r="F144" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -8034,13 +8136,16 @@
         <v>333</v>
       </c>
       <c r="B145" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C145" t="s">
         <v>1</v>
       </c>
       <c r="D145">
         <v>-1</v>
+      </c>
+      <c r="F145" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -8048,13 +8153,16 @@
         <v>334</v>
       </c>
       <c r="B146" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C146" t="s">
         <v>1</v>
       </c>
       <c r="D146">
         <v>-1</v>
+      </c>
+      <c r="F146" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -8073,6 +8181,9 @@
       <c r="E147" t="s">
         <v>133</v>
       </c>
+      <c r="F147" t="s">
+        <v>823</v>
+      </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
@@ -8087,19 +8198,25 @@
       <c r="D148">
         <v>-1</v>
       </c>
+      <c r="F148" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>337</v>
       </c>
       <c r="B149" t="s">
-        <v>620</v>
+        <v>816</v>
       </c>
       <c r="C149" t="s">
         <v>1</v>
       </c>
       <c r="D149">
         <v>-1</v>
+      </c>
+      <c r="F149" t="s">
+        <v>825</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -8118,27 +8235,30 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B151" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D151" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="E151" t="s">
         <v>133</v>
+      </c>
+      <c r="F151" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B152" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C152" t="s">
         <v>1</v>
@@ -8147,15 +8267,15 @@
         <v>-1</v>
       </c>
       <c r="F152" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B153" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C153" t="s">
         <v>1</v>
@@ -8164,15 +8284,15 @@
         <v>-1</v>
       </c>
       <c r="F153" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B154" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C154" t="s">
         <v>1</v>
@@ -8181,35 +8301,35 @@
         <v>-1</v>
       </c>
       <c r="F154" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
+        <v>737</v>
+      </c>
+      <c r="B155" t="s">
         <v>739</v>
       </c>
-      <c r="B155" t="s">
-        <v>741</v>
-      </c>
       <c r="C155" s="1" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D155" t="s">
+        <v>743</v>
+      </c>
+      <c r="F155" t="s">
         <v>745</v>
-      </c>
-      <c r="F155" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B156" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C156" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D156">
         <v>0</v>
@@ -8217,130 +8337,130 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B157" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C157" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D157" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E157" t="s">
         <v>133</v>
       </c>
       <c r="F157" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B158" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C158" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D158" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E158" t="s">
         <v>133</v>
       </c>
       <c r="F158" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B159" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C159" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D159" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E159" t="s">
         <v>133</v>
       </c>
       <c r="F159" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B160" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C160" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D160" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E160" t="s">
         <v>133</v>
       </c>
       <c r="F160" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B161" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C161" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D161" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E161" t="s">
         <v>133</v>
       </c>
       <c r="F161" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B162" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C162" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D162" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E162" t="s">
         <v>133</v>
       </c>
       <c r="F162" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B163" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C163" t="s">
         <v>1</v>
@@ -8349,15 +8469,15 @@
         <v>0</v>
       </c>
       <c r="F163" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>804</v>
+      </c>
+      <c r="B164" t="s">
         <v>806</v>
-      </c>
-      <c r="B164" t="s">
-        <v>808</v>
       </c>
       <c r="C164" t="s">
         <v>1</v>
@@ -8366,15 +8486,15 @@
         <v>0</v>
       </c>
       <c r="F164" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>805</v>
+      </c>
+      <c r="B165" t="s">
         <v>807</v>
-      </c>
-      <c r="B165" t="s">
-        <v>809</v>
       </c>
       <c r="C165" t="s">
         <v>1</v>
@@ -8383,7 +8503,7 @@
         <v>0</v>
       </c>
       <c r="F165" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
   </sheetData>
@@ -8396,7 +8516,7 @@
   <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8649,7 +8769,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C21" t="s">
         <v>143</v>
@@ -8660,7 +8780,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C22" t="s">
         <v>143</v>
@@ -8671,7 +8791,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C23" t="s">
         <v>143</v>
@@ -9826,7 +9946,7 @@
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
-        <v>817</v>
+        <v>827</v>
       </c>
       <c r="C128" t="s">
         <v>143</v>
@@ -9874,149 +9994,149 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B3" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E4" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B5" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E5" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B6" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E6" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B7" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E7" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B8" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E8" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B9" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E9" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B10" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -10024,13 +10144,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B11" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -10038,13 +10158,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B12" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -10052,13 +10172,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>779</v>
+      </c>
+      <c r="B13" t="s">
         <v>781</v>
       </c>
-      <c r="B13" t="s">
-        <v>783</v>
-      </c>
       <c r="C13" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -10066,13 +10186,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B14" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -10080,10 +10200,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B15" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>1</v>
@@ -10092,15 +10212,15 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B16" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>1</v>
@@ -10109,15 +10229,15 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B17" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>1</v>
@@ -10126,7 +10246,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename variable to make code more readable
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -2241,18 +2241,6 @@
     <t>Other VFD error</t>
   </si>
   <si>
-    <t>IO_airflowVfdStartStop</t>
-  </si>
-  <si>
-    <t>IO_airflowVfdFreqCmd</t>
-  </si>
-  <si>
-    <t>IO_airflowVfdInputSrc</t>
-  </si>
-  <si>
-    <t>IO_airflowVfdStatusMonitor</t>
-  </si>
-  <si>
     <t>D29000</t>
   </si>
   <si>
@@ -2521,6 +2509,18 @@
   </si>
   <si>
     <t>VENTILATION_VFD_STATUS_FLAG</t>
+  </si>
+  <si>
+    <t>Xfer_airflowVfdStartStop</t>
+  </si>
+  <si>
+    <t>Xfer_airflowVfdFreqCmd</t>
+  </si>
+  <si>
+    <t>Xfer_airflowVfdInputSrc</t>
+  </si>
+  <si>
+    <t>Xfer_airflowVfdStatusMonitor</t>
   </si>
 </sst>
 </file>
@@ -3969,7 +3969,7 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3984,7 +3984,7 @@
         <v>133</v>
       </c>
       <c r="G59" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
@@ -4109,7 +4109,7 @@
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -4124,12 +4124,12 @@
         <v>133</v>
       </c>
       <c r="G66" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -4144,12 +4144,12 @@
         <v>133</v>
       </c>
       <c r="G67" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -4164,12 +4164,12 @@
         <v>133</v>
       </c>
       <c r="G68" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -4184,12 +4184,12 @@
         <v>133</v>
       </c>
       <c r="G69" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -4204,7 +4204,7 @@
         <v>133</v>
       </c>
       <c r="G70" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
@@ -4400,7 +4400,7 @@
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -4412,12 +4412,12 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4432,12 +4432,12 @@
         <v>133</v>
       </c>
       <c r="G82" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -4452,7 +4452,7 @@
         <v>133</v>
       </c>
       <c r="G83" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.3">
@@ -5916,8 +5916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H144" sqref="H144"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F155" sqref="F155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7697,7 +7697,7 @@
         <v>-1</v>
       </c>
       <c r="F119" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -7714,7 +7714,7 @@
         <v>-1</v>
       </c>
       <c r="F120" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -7731,7 +7731,7 @@
         <v>-1</v>
       </c>
       <c r="F121" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -7748,7 +7748,7 @@
         <v>-1</v>
       </c>
       <c r="F122" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -7765,7 +7765,7 @@
         <v>-1</v>
       </c>
       <c r="F123" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -7782,7 +7782,7 @@
         <v>-1</v>
       </c>
       <c r="F124" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -7802,7 +7802,7 @@
         <v>133</v>
       </c>
       <c r="F125" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -7819,7 +7819,7 @@
         <v>-1</v>
       </c>
       <c r="F126" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -7836,7 +7836,7 @@
         <v>-1</v>
       </c>
       <c r="F127" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -7870,7 +7870,7 @@
         <v>133</v>
       </c>
       <c r="F129" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -7887,7 +7887,7 @@
         <v>-1</v>
       </c>
       <c r="F130" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -7904,7 +7904,7 @@
         <v>-1</v>
       </c>
       <c r="F131" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -7921,7 +7921,7 @@
         <v>-1</v>
       </c>
       <c r="F132" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -7938,7 +7938,7 @@
         <v>-1</v>
       </c>
       <c r="F133" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -7955,7 +7955,7 @@
         <v>-1</v>
       </c>
       <c r="F134" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -7972,7 +7972,7 @@
         <v>-1</v>
       </c>
       <c r="F135" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -7992,7 +7992,7 @@
         <v>133</v>
       </c>
       <c r="F136" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -8009,7 +8009,7 @@
         <v>-1</v>
       </c>
       <c r="F137" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -8017,7 +8017,7 @@
         <v>327</v>
       </c>
       <c r="B138" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C138" t="s">
         <v>1</v>
@@ -8026,7 +8026,7 @@
         <v>-1</v>
       </c>
       <c r="F138" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -8060,7 +8060,7 @@
         <v>133</v>
       </c>
       <c r="F140" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -8077,7 +8077,7 @@
         <v>-1</v>
       </c>
       <c r="F141" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -8094,7 +8094,7 @@
         <v>-1</v>
       </c>
       <c r="F142" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -8111,7 +8111,7 @@
         <v>-1</v>
       </c>
       <c r="F143" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -8128,7 +8128,7 @@
         <v>-1</v>
       </c>
       <c r="F144" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -8145,7 +8145,7 @@
         <v>-1</v>
       </c>
       <c r="F145" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -8162,7 +8162,7 @@
         <v>-1</v>
       </c>
       <c r="F146" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -8182,7 +8182,7 @@
         <v>133</v>
       </c>
       <c r="F147" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -8199,7 +8199,7 @@
         <v>-1</v>
       </c>
       <c r="F148" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -8207,7 +8207,7 @@
         <v>337</v>
       </c>
       <c r="B149" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C149" t="s">
         <v>1</v>
@@ -8216,7 +8216,7 @@
         <v>-1</v>
       </c>
       <c r="F149" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -8250,16 +8250,16 @@
         <v>133</v>
       </c>
       <c r="F151" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
+        <v>824</v>
+      </c>
+      <c r="B152" t="s">
         <v>734</v>
       </c>
-      <c r="B152" t="s">
-        <v>738</v>
-      </c>
       <c r="C152" t="s">
         <v>1</v>
       </c>
@@ -8267,32 +8267,32 @@
         <v>-1</v>
       </c>
       <c r="F152" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>735</v>
+        <v>825</v>
       </c>
       <c r="B153" t="s">
+        <v>736</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>-1</v>
+      </c>
+      <c r="F153" t="s">
         <v>740</v>
-      </c>
-      <c r="C153" t="s">
-        <v>1</v>
-      </c>
-      <c r="D153">
-        <v>-1</v>
-      </c>
-      <c r="F153" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>736</v>
+        <v>826</v>
       </c>
       <c r="B154" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C154" t="s">
         <v>1</v>
@@ -8301,24 +8301,24 @@
         <v>-1</v>
       </c>
       <c r="F154" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>737</v>
+        <v>827</v>
       </c>
       <c r="B155" t="s">
+        <v>735</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="D155" t="s">
         <v>739</v>
       </c>
-      <c r="C155" s="1" t="s">
-        <v>742</v>
-      </c>
-      <c r="D155" t="s">
-        <v>743</v>
-      </c>
       <c r="F155" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -8340,7 +8340,7 @@
         <v>698</v>
       </c>
       <c r="B157" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="C157" t="s">
         <v>708</v>
@@ -8360,7 +8360,7 @@
         <v>701</v>
       </c>
       <c r="B158" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C158" t="s">
         <v>708</v>
@@ -8380,7 +8380,7 @@
         <v>699</v>
       </c>
       <c r="B159" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C159" t="s">
         <v>708</v>
@@ -8400,7 +8400,7 @@
         <v>700</v>
       </c>
       <c r="B160" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="C160" t="s">
         <v>708</v>
@@ -8420,7 +8420,7 @@
         <v>694</v>
       </c>
       <c r="B161" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="C161" t="s">
         <v>708</v>
@@ -8440,7 +8440,7 @@
         <v>696</v>
       </c>
       <c r="B162" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="C162" t="s">
         <v>708</v>
@@ -8457,10 +8457,10 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="B163" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="C163" t="s">
         <v>1</v>
@@ -8469,15 +8469,15 @@
         <v>0</v>
       </c>
       <c r="F163" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="B164" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="C164" t="s">
         <v>1</v>
@@ -8486,15 +8486,15 @@
         <v>0</v>
       </c>
       <c r="F164" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B165" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C165" t="s">
         <v>1</v>
@@ -8503,7 +8503,7 @@
         <v>0</v>
       </c>
       <c r="F165" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
   </sheetData>
@@ -8515,7 +8515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
@@ -9946,7 +9946,7 @@
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C128" t="s">
         <v>143</v>
@@ -10006,7 +10006,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -10014,7 +10014,7 @@
         <v>702</v>
       </c>
       <c r="B3" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>637</v>
@@ -10023,15 +10023,15 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>745</v>
+      </c>
+      <c r="B4" t="s">
         <v>749</v>
-      </c>
-      <c r="B4" t="s">
-        <v>753</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>708</v>
@@ -10040,15 +10040,15 @@
         <v>707</v>
       </c>
       <c r="E4" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="B5" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>708</v>
@@ -10057,15 +10057,15 @@
         <v>707</v>
       </c>
       <c r="E5" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="B6" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>708</v>
@@ -10074,15 +10074,15 @@
         <v>707</v>
       </c>
       <c r="E6" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B7" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>708</v>
@@ -10091,7 +10091,7 @@
         <v>707</v>
       </c>
       <c r="E7" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -10099,7 +10099,7 @@
         <v>694</v>
       </c>
       <c r="B8" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>708</v>
@@ -10108,7 +10108,7 @@
         <v>707</v>
       </c>
       <c r="E8" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -10116,7 +10116,7 @@
         <v>696</v>
       </c>
       <c r="B9" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>708</v>
@@ -10125,15 +10125,15 @@
         <v>707</v>
       </c>
       <c r="E9" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B10" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>637</v>
@@ -10144,10 +10144,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B11" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>637</v>
@@ -10158,10 +10158,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B12" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>637</v>
@@ -10172,10 +10172,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B13" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>637</v>
@@ -10186,10 +10186,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>776</v>
+      </c>
+      <c r="B14" t="s">
         <v>780</v>
-      </c>
-      <c r="B14" t="s">
-        <v>784</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>637</v>
@@ -10200,10 +10200,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="B15" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>1</v>
@@ -10212,15 +10212,15 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B16" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>1</v>
@@ -10229,15 +10229,15 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="B17" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>1</v>
@@ -10246,7 +10246,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new display in HMI.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="828">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -5917,7 +5917,7 @@
   <dimension ref="A1:F165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A135" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F155" sqref="F155"/>
+      <selection activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8316,6 +8316,9 @@
       </c>
       <c r="D155" t="s">
         <v>739</v>
+      </c>
+      <c r="E155" t="s">
+        <v>133</v>
       </c>
       <c r="F155" t="s">
         <v>741</v>

</xml_diff>

<commit_message>
Added more check for SM flags in PLC2.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="14376" windowHeight="10500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="834">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2521,6 +2521,24 @@
   </si>
   <si>
     <t>Xfer_airflowVfdStatusMonitor</t>
+  </si>
+  <si>
+    <t>errorCOM</t>
+  </si>
+  <si>
+    <t>D3003</t>
+  </si>
+  <si>
+    <t>Error in the COM port (ventilation sensors)</t>
+  </si>
+  <si>
+    <t>errorPLC2com</t>
+  </si>
+  <si>
+    <t>D27003</t>
+  </si>
+  <si>
+    <t>PLC2 COM error</t>
   </si>
 </sst>
 </file>
@@ -2879,7 +2897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
@@ -5914,10 +5932,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F165"/>
+  <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E156" sqref="E156"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F167" sqref="F167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8507,6 +8525,23 @@
       </c>
       <c r="F165" t="s">
         <v>806</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>831</v>
+      </c>
+      <c r="B166" t="s">
+        <v>832</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="F166" t="s">
+        <v>833</v>
       </c>
     </row>
   </sheetData>
@@ -9965,10 +10000,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10252,6 +10287,23 @@
         <v>799</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>828</v>
+      </c>
+      <c r="B18" t="s">
+        <v>829</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>830</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Use internal timer (SM396) instead of counter
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -2982,10 +2982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4764,6 +4764,12 @@
       <c r="G94" t="s">
         <v>857</v>
       </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D95" s="8"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D96" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement separate flowrate setting for each of the sections instead of one setting for all.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="867">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2626,6 +2626,18 @@
   </si>
   <si>
     <t>Bad sectors</t>
+  </si>
+  <si>
+    <t>[3(32)]</t>
+  </si>
+  <si>
+    <t>flowratePerShelf_local</t>
+  </si>
+  <si>
+    <t>pumpFillDrainCountDownTimer_s</t>
+  </si>
+  <si>
+    <t>Countdown timer</t>
   </si>
 </sst>
 </file>
@@ -2984,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3476,7 +3488,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>630</v>
+        <v>864</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3484,11 +3496,8 @@
       <c r="D27" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="7">
         <v>32</v>
-      </c>
-      <c r="F27" t="s">
-        <v>133</v>
       </c>
       <c r="G27" t="s">
         <v>619</v>
@@ -4766,10 +4775,44 @@
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D95" s="8"/>
+      <c r="B95" t="s">
+        <v>630</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>863</v>
+      </c>
+      <c r="F95" t="s">
+        <v>133</v>
+      </c>
+      <c r="G95" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D96" s="8"/>
+      <c r="B96" t="s">
+        <v>865</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E96" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" t="s">
+        <v>133</v>
+      </c>
+      <c r="G96" t="s">
+        <v>866</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement pump error check for scenario where pump would run too fast, eg. lacks water. In case of error for 15s, motor will be stopped
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="871">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2638,6 +2638,18 @@
   </si>
   <si>
     <t>Countdown timer</t>
+  </si>
+  <si>
+    <t>pumpAbnormalFlag</t>
+  </si>
+  <si>
+    <t>pumpAbnormalityStartTime</t>
+  </si>
+  <si>
+    <t>Flag idicate something is abnormal</t>
+  </si>
+  <si>
+    <t>Anormality start time</t>
   </si>
 </sst>
 </file>
@@ -2994,10 +3006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G97" sqref="G97"/>
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4812,6 +4824,43 @@
       </c>
       <c r="G96" t="s">
         <v>866</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>867</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E97" t="s">
+        <v>0</v>
+      </c>
+      <c r="F97" t="s">
+        <v>133</v>
+      </c>
+      <c r="G97" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>868</v>
+      </c>
+      <c r="C98">
+        <v>3</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" t="s">
+        <v>870</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix and tested motor disabling flags.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="873">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2646,10 +2646,16 @@
     <t>pumpAbnormalityStartTime</t>
   </si>
   <si>
-    <t>Flag idicate something is abnormal</t>
-  </si>
-  <si>
     <t>Anormality start time</t>
+  </si>
+  <si>
+    <t>pumpAbnormalTermination</t>
+  </si>
+  <si>
+    <t>Flag indicate something is abnormal</t>
+  </si>
+  <si>
+    <t>Pump stopped due to prolonged abnormality</t>
   </si>
 </sst>
 </file>
@@ -3006,10 +3012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4843,7 +4849,7 @@
         <v>133</v>
       </c>
       <c r="G97" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
@@ -4860,7 +4866,27 @@
         <v>12</v>
       </c>
       <c r="G98" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
         <v>870</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E99" t="s">
+        <v>0</v>
+      </c>
+      <c r="F99" t="s">
+        <v>133</v>
+      </c>
+      <c r="G99" t="s">
+        <v>872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added water temperature offset. Note that there is a python script bug that causes the csv generator to fail. Have to edit the csv file manually to fix the issue. Python script will be fix in another task.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="890">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2656,6 +2656,57 @@
   </si>
   <si>
     <t>Pump stopped due to prolonged abnormality</t>
+  </si>
+  <si>
+    <t>pumpTerminationThreshold_hz</t>
+  </si>
+  <si>
+    <t>Pump threshold in hz before termination</t>
+  </si>
+  <si>
+    <t>Overflow timer</t>
+  </si>
+  <si>
+    <t>Overflow last reading of SR396 used to determine whether 1 second has elapsed</t>
+  </si>
+  <si>
+    <t>overflow_last_time</t>
+  </si>
+  <si>
+    <t>overflow_counter</t>
+  </si>
+  <si>
+    <t>waterTempOffset</t>
+  </si>
+  <si>
+    <t>[20(0)]</t>
+  </si>
+  <si>
+    <t>Offset to water temperature</t>
+  </si>
+  <si>
+    <t>waterTempOffsetNegative</t>
+  </si>
+  <si>
+    <t>ARRAY [20] OF WORD</t>
+  </si>
+  <si>
+    <t>ARRAY [20] OF BOOL</t>
+  </si>
+  <si>
+    <t>[20(FALSE)]</t>
+  </si>
+  <si>
+    <t>True if negative offset</t>
+  </si>
+  <si>
+    <t>waterTempFinal</t>
+  </si>
+  <si>
+    <t>Water temp after offset is included</t>
+  </si>
+  <si>
+    <t>retain</t>
   </si>
 </sst>
 </file>
@@ -3012,10 +3063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H103" sqref="H103:H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3025,10 +3076,10 @@
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -3050,8 +3101,11 @@
       <c r="G1" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20000</v>
       </c>
@@ -3074,7 +3128,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>25</v>
       </c>
@@ -3089,7 +3143,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -3103,7 +3157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>352</v>
       </c>
@@ -3123,7 +3177,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>353</v>
       </c>
@@ -3140,7 +3194,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>354</v>
       </c>
@@ -3157,7 +3211,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>355</v>
       </c>
@@ -3174,7 +3228,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>359</v>
       </c>
@@ -3191,7 +3245,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>356</v>
       </c>
@@ -3208,7 +3262,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>357</v>
       </c>
@@ -3225,7 +3279,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>501</v>
       </c>
@@ -3242,7 +3296,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>405</v>
       </c>
@@ -3259,7 +3313,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>358</v>
       </c>
@@ -3276,7 +3330,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>369</v>
       </c>
@@ -3293,7 +3347,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>383</v>
       </c>
@@ -4888,6 +4942,126 @@
       <c r="G99" t="s">
         <v>872</v>
       </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>873</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <v>45</v>
+      </c>
+      <c r="F100" t="s">
+        <v>133</v>
+      </c>
+      <c r="G100" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>877</v>
+      </c>
+      <c r="C101">
+        <v>10</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E101" t="s">
+        <v>647</v>
+      </c>
+      <c r="G101" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>878</v>
+      </c>
+      <c r="C102">
+        <v>10</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>647</v>
+      </c>
+      <c r="G102" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>879</v>
+      </c>
+      <c r="C103">
+        <v>20</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>883</v>
+      </c>
+      <c r="E103" t="s">
+        <v>880</v>
+      </c>
+      <c r="F103" t="s">
+        <v>133</v>
+      </c>
+      <c r="G103" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>882</v>
+      </c>
+      <c r="C104">
+        <v>20</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>884</v>
+      </c>
+      <c r="E104" t="s">
+        <v>885</v>
+      </c>
+      <c r="F104" t="s">
+        <v>133</v>
+      </c>
+      <c r="G104" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>887</v>
+      </c>
+      <c r="C105">
+        <v>20</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>883</v>
+      </c>
+      <c r="E105" t="s">
+        <v>880</v>
+      </c>
+      <c r="F105" t="s">
+        <v>133</v>
+      </c>
+      <c r="G105" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D106" s="8"/>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D107" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4899,7 +5073,7 @@
   <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4938,6 +5112,9 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>351</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>889</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5938,10 +6115,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5954,7 +6131,7 @@
     <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -5976,8 +6153,11 @@
       <c r="G1" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>350</v>
       </c>
@@ -5994,7 +6174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -6009,7 +6189,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -6023,7 +6203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -6037,7 +6217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -6051,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -6065,7 +6245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
     </row>
   </sheetData>
@@ -6075,10 +6255,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6091,7 +6271,7 @@
     <col min="7" max="7" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -6113,8 +6293,11 @@
       <c r="G1" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11000</v>
       </c>
@@ -6134,7 +6317,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>138</v>
       </c>
@@ -6151,7 +6334,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>137</v>
       </c>
@@ -6171,7 +6354,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>624</v>
       </c>
@@ -6188,7 +6371,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>139</v>
       </c>
@@ -6205,7 +6388,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>345</v>
       </c>
@@ -6222,7 +6405,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>140</v>
       </c>
@@ -6239,7 +6422,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>141</v>
       </c>
@@ -6256,7 +6439,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>626</v>
       </c>
@@ -6273,7 +6456,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>627</v>
       </c>
@@ -6290,7 +6473,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>628</v>
       </c>
@@ -6307,7 +6490,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>629</v>
       </c>
@@ -6324,7 +6507,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
     </row>
   </sheetData>
@@ -6334,10 +6517,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152:F152"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6349,7 +6532,7 @@
     <col min="6" max="6" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -6368,8 +6551,11 @@
       <c r="F1" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -6383,7 +6569,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>152</v>
       </c>
@@ -6397,7 +6583,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>153</v>
       </c>
@@ -6411,7 +6597,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -6425,7 +6611,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>157</v>
       </c>
@@ -6439,7 +6625,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>158</v>
       </c>
@@ -6453,7 +6639,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -6467,7 +6653,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -6481,7 +6667,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -6495,7 +6681,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>161</v>
       </c>
@@ -6509,7 +6695,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -6523,7 +6709,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -6537,7 +6723,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>163</v>
       </c>
@@ -6551,7 +6737,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>164</v>
       </c>
@@ -6565,7 +6751,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>165</v>
       </c>
@@ -8972,8 +9158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B134" sqref="B134"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9001,6 +9187,9 @@
       <c r="E1" t="s">
         <v>351</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>889</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -10485,10 +10674,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10498,7 +10687,7 @@
     <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
@@ -10514,8 +10703,11 @@
       <c r="E1" s="9" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>693</v>
       </c>
@@ -10532,7 +10724,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>702</v>
       </c>
@@ -10549,7 +10741,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>745</v>
       </c>
@@ -10566,7 +10758,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>746</v>
       </c>
@@ -10583,7 +10775,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>747</v>
       </c>
@@ -10600,7 +10792,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>748</v>
       </c>
@@ -10617,7 +10809,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>694</v>
       </c>
@@ -10634,7 +10826,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>696</v>
       </c>
@@ -10651,7 +10843,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>771</v>
       </c>
@@ -10665,7 +10857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>778</v>
       </c>
@@ -10679,7 +10871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>779</v>
       </c>
@@ -10693,7 +10885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>775</v>
       </c>
@@ -10707,7 +10899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>776</v>
       </c>
@@ -10721,7 +10913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>781</v>
       </c>
@@ -10738,7 +10930,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>794</v>
       </c>

</xml_diff>

<commit_message>
HMI only code change. Allow non-stop water or light while in auto mode. Theoretically complete, but not tested.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="930">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2707,6 +2707,126 @@
   </si>
   <si>
     <t>retain</t>
+  </si>
+  <si>
+    <t>S0_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S0_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S1_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S1_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S2_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S2_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S3_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S3_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S4_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S4_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S5_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S5_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S6_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S6_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S7_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S7_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S8_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S8_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S9_WATER_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S9_WATER_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S0_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S0_LIGHT_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S1_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S1_LIGHT_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S2_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S2_LIGHT_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S3_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S3_LIGHT_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S4_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S4_LIGHT_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S5_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S5_LIGHT_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S6_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S6_LIGHT_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S7_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S7_LIGHT_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S8_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S8_LIGHT_ALWAYS_ON</t>
+  </si>
+  <si>
+    <t>S9_LIGHT_IGNORE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>S9_LIGHT_ALWAYS_ON</t>
   </si>
 </sst>
 </file>
@@ -3065,8 +3185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H103" sqref="H103:H104"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9156,10 +9276,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G134"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9454,7 +9574,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -9536,10 +9656,10 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>411</v>
+        <v>890</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -9547,10 +9667,10 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>412</v>
+        <v>891</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -9558,7 +9678,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -9569,7 +9689,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -9580,7 +9700,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -9591,7 +9711,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -9602,10 +9722,10 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>419</v>
+        <v>910</v>
       </c>
       <c r="C38" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -9613,10 +9733,10 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>420</v>
+        <v>911</v>
       </c>
       <c r="C39" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -9624,7 +9744,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -9635,7 +9755,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
@@ -9646,7 +9766,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -9657,7 +9777,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -9668,10 +9788,10 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>425</v>
+        <v>892</v>
       </c>
       <c r="C44" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -9679,10 +9799,10 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>426</v>
+        <v>893</v>
       </c>
       <c r="C45" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -9690,7 +9810,7 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
@@ -9701,7 +9821,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
@@ -9712,7 +9832,7 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
@@ -9723,7 +9843,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
@@ -9734,10 +9854,10 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>431</v>
+        <v>912</v>
       </c>
       <c r="C50" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -9745,10 +9865,10 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>432</v>
+        <v>913</v>
       </c>
       <c r="C51" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -9756,7 +9876,7 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -9767,7 +9887,7 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
@@ -9778,7 +9898,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
@@ -9789,7 +9909,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
@@ -9800,10 +9920,10 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>437</v>
+        <v>894</v>
       </c>
       <c r="C56" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -9811,10 +9931,10 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>438</v>
+        <v>895</v>
       </c>
       <c r="C57" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -9822,7 +9942,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
@@ -9833,7 +9953,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -9844,7 +9964,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
@@ -9855,7 +9975,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
@@ -9866,10 +9986,10 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>443</v>
+        <v>914</v>
       </c>
       <c r="C62" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -9877,10 +9997,10 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>444</v>
+        <v>915</v>
       </c>
       <c r="C63" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -9888,7 +10008,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
@@ -9899,7 +10019,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
@@ -9910,7 +10030,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
@@ -9921,7 +10041,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
@@ -9932,10 +10052,10 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>449</v>
+        <v>896</v>
       </c>
       <c r="C68" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -9943,10 +10063,10 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>450</v>
+        <v>897</v>
       </c>
       <c r="C69" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -9954,7 +10074,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
@@ -9965,7 +10085,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
@@ -9976,7 +10096,7 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
@@ -9987,7 +10107,7 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
@@ -9998,10 +10118,10 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>455</v>
+        <v>916</v>
       </c>
       <c r="C74" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -10009,10 +10129,10 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>456</v>
+        <v>917</v>
       </c>
       <c r="C75" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -10020,7 +10140,7 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
@@ -10031,7 +10151,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
@@ -10042,7 +10162,7 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
@@ -10053,7 +10173,7 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
@@ -10064,10 +10184,10 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>461</v>
+        <v>898</v>
       </c>
       <c r="C80" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -10075,10 +10195,10 @@
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>462</v>
+        <v>899</v>
       </c>
       <c r="C81" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -10086,7 +10206,7 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
@@ -10097,7 +10217,7 @@
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
@@ -10108,7 +10228,7 @@
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
@@ -10119,7 +10239,7 @@
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
@@ -10130,10 +10250,10 @@
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>467</v>
+        <v>918</v>
       </c>
       <c r="C86" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -10141,10 +10261,10 @@
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>468</v>
+        <v>919</v>
       </c>
       <c r="C87" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -10152,7 +10272,7 @@
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>469</v>
+        <v>449</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
@@ -10163,7 +10283,7 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
@@ -10174,7 +10294,7 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>471</v>
+        <v>451</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
@@ -10185,7 +10305,7 @@
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>472</v>
+        <v>452</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
@@ -10196,10 +10316,10 @@
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>473</v>
+        <v>900</v>
       </c>
       <c r="C92" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -10207,10 +10327,10 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>474</v>
+        <v>901</v>
       </c>
       <c r="C93" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -10218,7 +10338,7 @@
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>475</v>
+        <v>453</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
@@ -10229,7 +10349,7 @@
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>476</v>
+        <v>454</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
@@ -10240,7 +10360,7 @@
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>477</v>
+        <v>455</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
@@ -10251,7 +10371,7 @@
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>478</v>
+        <v>456</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
@@ -10262,10 +10382,10 @@
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>479</v>
+        <v>920</v>
       </c>
       <c r="C98" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -10273,10 +10393,10 @@
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>480</v>
+        <v>921</v>
       </c>
       <c r="C99" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -10284,7 +10404,7 @@
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
@@ -10295,7 +10415,7 @@
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
@@ -10306,7 +10426,7 @@
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
@@ -10317,7 +10437,7 @@
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
@@ -10328,10 +10448,10 @@
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>485</v>
+        <v>902</v>
       </c>
       <c r="C104" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -10339,10 +10459,10 @@
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>486</v>
+        <v>903</v>
       </c>
       <c r="C105" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -10350,7 +10470,7 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
@@ -10361,7 +10481,7 @@
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>488</v>
+        <v>462</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
@@ -10372,7 +10492,7 @@
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>581</v>
+        <v>463</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
@@ -10383,7 +10503,7 @@
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>582</v>
+        <v>464</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
@@ -10394,10 +10514,10 @@
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>583</v>
+        <v>922</v>
       </c>
       <c r="C110" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -10405,10 +10525,10 @@
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>584</v>
+        <v>923</v>
       </c>
       <c r="C111" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -10416,7 +10536,7 @@
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>585</v>
+        <v>465</v>
       </c>
       <c r="C112" t="s">
         <v>1</v>
@@ -10427,7 +10547,7 @@
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>586</v>
+        <v>466</v>
       </c>
       <c r="C113" t="s">
         <v>1</v>
@@ -10438,7 +10558,7 @@
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>587</v>
+        <v>467</v>
       </c>
       <c r="C114" t="s">
         <v>1</v>
@@ -10449,7 +10569,7 @@
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>588</v>
+        <v>468</v>
       </c>
       <c r="C115" t="s">
         <v>1</v>
@@ -10460,10 +10580,10 @@
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>589</v>
+        <v>904</v>
       </c>
       <c r="C116" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -10471,10 +10591,10 @@
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>590</v>
+        <v>905</v>
       </c>
       <c r="C117" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -10482,7 +10602,7 @@
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>591</v>
+        <v>469</v>
       </c>
       <c r="C118" t="s">
         <v>1</v>
@@ -10493,7 +10613,7 @@
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>592</v>
+        <v>470</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
@@ -10504,7 +10624,7 @@
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>593</v>
+        <v>471</v>
       </c>
       <c r="C120" t="s">
         <v>1</v>
@@ -10515,7 +10635,7 @@
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>594</v>
+        <v>472</v>
       </c>
       <c r="C121" t="s">
         <v>1</v>
@@ -10526,10 +10646,10 @@
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>595</v>
+        <v>924</v>
       </c>
       <c r="C122" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -10537,10 +10657,10 @@
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>596</v>
+        <v>925</v>
       </c>
       <c r="C123" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D123">
         <v>1</v>
@@ -10548,7 +10668,7 @@
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>597</v>
+        <v>473</v>
       </c>
       <c r="C124" t="s">
         <v>1</v>
@@ -10559,7 +10679,7 @@
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>598</v>
+        <v>474</v>
       </c>
       <c r="C125" t="s">
         <v>1</v>
@@ -10570,7 +10690,7 @@
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>599</v>
+        <v>475</v>
       </c>
       <c r="C126" t="s">
         <v>1</v>
@@ -10581,7 +10701,7 @@
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>600</v>
+        <v>476</v>
       </c>
       <c r="C127" t="s">
         <v>1</v>
@@ -10592,7 +10712,7 @@
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>823</v>
+        <v>906</v>
       </c>
       <c r="C128" t="s">
         <v>143</v>
@@ -10603,10 +10723,10 @@
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>844</v>
+        <v>907</v>
       </c>
       <c r="C129" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -10614,7 +10734,7 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>845</v>
+        <v>477</v>
       </c>
       <c r="C130" t="s">
         <v>1</v>
@@ -10625,7 +10745,7 @@
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>846</v>
+        <v>478</v>
       </c>
       <c r="C131" t="s">
         <v>1</v>
@@ -10636,7 +10756,7 @@
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>847</v>
+        <v>479</v>
       </c>
       <c r="C132" t="s">
         <v>1</v>
@@ -10647,7 +10767,7 @@
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>849</v>
+        <v>480</v>
       </c>
       <c r="C133" t="s">
         <v>1</v>
@@ -10658,12 +10778,452 @@
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>860</v>
+        <v>926</v>
       </c>
       <c r="C134" t="s">
         <v>143</v>
       </c>
       <c r="D134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>927</v>
+      </c>
+      <c r="C135" t="s">
+        <v>143</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>481</v>
+      </c>
+      <c r="C136" t="s">
+        <v>1</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>482</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>483</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>484</v>
+      </c>
+      <c r="C139" t="s">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>908</v>
+      </c>
+      <c r="C140" t="s">
+        <v>143</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>909</v>
+      </c>
+      <c r="C141" t="s">
+        <v>143</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>485</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>486</v>
+      </c>
+      <c r="C143" t="s">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>487</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>488</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>928</v>
+      </c>
+      <c r="C146" t="s">
+        <v>143</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>929</v>
+      </c>
+      <c r="C147" t="s">
+        <v>143</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>581</v>
+      </c>
+      <c r="C148" t="s">
+        <v>1</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>582</v>
+      </c>
+      <c r="C149" t="s">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>583</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>584</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>585</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>586</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>587</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>588</v>
+      </c>
+      <c r="C155" t="s">
+        <v>1</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>589</v>
+      </c>
+      <c r="C156" t="s">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>590</v>
+      </c>
+      <c r="C157" t="s">
+        <v>1</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>591</v>
+      </c>
+      <c r="C158" t="s">
+        <v>1</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>592</v>
+      </c>
+      <c r="C159" t="s">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>593</v>
+      </c>
+      <c r="C160" t="s">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>594</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>595</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>596</v>
+      </c>
+      <c r="C163" t="s">
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>597</v>
+      </c>
+      <c r="C164" t="s">
+        <v>1</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>598</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>599</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>600</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>823</v>
+      </c>
+      <c r="C168" t="s">
+        <v>143</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>844</v>
+      </c>
+      <c r="C169" t="s">
+        <v>1</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>845</v>
+      </c>
+      <c r="C170" t="s">
+        <v>1</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>846</v>
+      </c>
+      <c r="C171" t="s">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>847</v>
+      </c>
+      <c r="C172" t="s">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>849</v>
+      </c>
+      <c r="C173" t="s">
+        <v>1</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>860</v>
+      </c>
+      <c r="C174" t="s">
+        <v>143</v>
+      </c>
+      <c r="D174">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix schedule bug by removing the code that enables water and light to be independent in auto mode.
</commit_message>
<xml_diff>
--- a/rack_control/global_variable_template.xlsx
+++ b/rack_control/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="908">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2680,126 +2680,6 @@
   </si>
   <si>
     <t>retain</t>
-  </si>
-  <si>
-    <t>S0_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S0_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S1_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S1_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S2_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S2_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S3_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S3_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S4_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S4_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S5_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S5_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S6_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S6_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S7_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S7_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S8_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S8_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S9_WATER_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S9_WATER_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S0_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S0_LIGHT_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S1_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S1_LIGHT_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S2_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S2_LIGHT_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S3_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S3_LIGHT_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S4_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S4_LIGHT_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S5_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S5_LIGHT_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S6_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S6_LIGHT_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S7_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S7_LIGHT_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S8_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S8_LIGHT_ALWAYS_ON</t>
-  </si>
-  <si>
-    <t>S9_LIGHT_IGNORE_SCHEDULE</t>
-  </si>
-  <si>
-    <t>S9_LIGHT_ALWAYS_ON</t>
   </si>
   <si>
     <t>overflowLocal</t>
@@ -5233,22 +5113,22 @@
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>921</v>
+        <v>881</v>
       </c>
       <c r="C106">
         <v>10</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>923</v>
+        <v>883</v>
       </c>
       <c r="E106" t="s">
-        <v>922</v>
+        <v>882</v>
       </c>
       <c r="F106" t="s">
         <v>133</v>
       </c>
       <c r="G106" t="s">
-        <v>924</v>
+        <v>884</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
@@ -7616,7 +7496,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>925</v>
+        <v>885</v>
       </c>
       <c r="B64" t="s">
         <v>273</v>
@@ -7631,12 +7511,12 @@
         <v>133</v>
       </c>
       <c r="F64" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>926</v>
+        <v>886</v>
       </c>
       <c r="B65" t="s">
         <v>274</v>
@@ -7651,12 +7531,12 @@
         <v>133</v>
       </c>
       <c r="F65" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>927</v>
+        <v>887</v>
       </c>
       <c r="B66" t="s">
         <v>275</v>
@@ -7671,12 +7551,12 @@
         <v>133</v>
       </c>
       <c r="F66" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>928</v>
+        <v>888</v>
       </c>
       <c r="B67" t="s">
         <v>276</v>
@@ -7691,12 +7571,12 @@
         <v>133</v>
       </c>
       <c r="F67" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>929</v>
+        <v>889</v>
       </c>
       <c r="B68" t="s">
         <v>277</v>
@@ -7711,12 +7591,12 @@
         <v>133</v>
       </c>
       <c r="F68" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>930</v>
+        <v>890</v>
       </c>
       <c r="B69" t="s">
         <v>278</v>
@@ -7731,12 +7611,12 @@
         <v>133</v>
       </c>
       <c r="F69" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>931</v>
+        <v>891</v>
       </c>
       <c r="B70" t="s">
         <v>279</v>
@@ -7751,12 +7631,12 @@
         <v>133</v>
       </c>
       <c r="F70" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>932</v>
+        <v>892</v>
       </c>
       <c r="B71" t="s">
         <v>280</v>
@@ -7771,15 +7651,15 @@
         <v>133</v>
       </c>
       <c r="F71" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>933</v>
+        <v>893</v>
       </c>
       <c r="B72" t="s">
-        <v>935</v>
+        <v>895</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
@@ -7791,15 +7671,15 @@
         <v>133</v>
       </c>
       <c r="F72" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>934</v>
+        <v>894</v>
       </c>
       <c r="B73" t="s">
-        <v>936</v>
+        <v>896</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
@@ -7811,7 +7691,7 @@
         <v>133</v>
       </c>
       <c r="F73" t="s">
-        <v>937</v>
+        <v>897</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -9399,10 +9279,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G184"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="B185" sqref="B185"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9697,7 +9577,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -9779,10 +9659,10 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>881</v>
+        <v>403</v>
       </c>
       <c r="C32" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -9790,10 +9670,10 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>882</v>
+        <v>404</v>
       </c>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -9801,7 +9681,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -9812,7 +9692,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -9823,7 +9703,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -9834,7 +9714,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -9845,10 +9725,10 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>901</v>
+        <v>411</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -9856,10 +9736,10 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>902</v>
+        <v>412</v>
       </c>
       <c r="C39" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -9867,7 +9747,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -9878,7 +9758,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
@@ -9889,7 +9769,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -9900,7 +9780,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -9911,10 +9791,10 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>883</v>
+        <v>417</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -9922,10 +9802,10 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>884</v>
+        <v>418</v>
       </c>
       <c r="C45" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -9933,7 +9813,7 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
@@ -9944,7 +9824,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
@@ -9955,7 +9835,7 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
@@ -9966,7 +9846,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
@@ -9977,10 +9857,10 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>903</v>
+        <v>423</v>
       </c>
       <c r="C50" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -9988,10 +9868,10 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>904</v>
+        <v>424</v>
       </c>
       <c r="C51" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -9999,7 +9879,7 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -10010,7 +9890,7 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
@@ -10021,7 +9901,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
@@ -10032,7 +9912,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
@@ -10043,10 +9923,10 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>885</v>
+        <v>429</v>
       </c>
       <c r="C56" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -10054,10 +9934,10 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>886</v>
+        <v>430</v>
       </c>
       <c r="C57" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -10065,7 +9945,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
@@ -10076,7 +9956,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -10087,7 +9967,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
@@ -10098,7 +9978,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
@@ -10109,10 +9989,10 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>905</v>
+        <v>435</v>
       </c>
       <c r="C62" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -10120,10 +10000,10 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>906</v>
+        <v>436</v>
       </c>
       <c r="C63" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -10131,7 +10011,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
@@ -10142,7 +10022,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
@@ -10153,7 +10033,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
@@ -10164,7 +10044,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
@@ -10175,10 +10055,10 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>887</v>
+        <v>441</v>
       </c>
       <c r="C68" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -10186,10 +10066,10 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>888</v>
+        <v>442</v>
       </c>
       <c r="C69" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -10197,7 +10077,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>429</v>
+        <v>443</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
@@ -10208,7 +10088,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
@@ -10219,7 +10099,7 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
@@ -10230,7 +10110,7 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
@@ -10241,10 +10121,10 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>907</v>
+        <v>447</v>
       </c>
       <c r="C74" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -10252,10 +10132,10 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>908</v>
+        <v>448</v>
       </c>
       <c r="C75" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -10263,7 +10143,7 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>433</v>
+        <v>449</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
@@ -10274,7 +10154,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>434</v>
+        <v>450</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
@@ -10285,7 +10165,7 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>435</v>
+        <v>451</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
@@ -10296,7 +10176,7 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>436</v>
+        <v>452</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
@@ -10307,10 +10187,10 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>889</v>
+        <v>453</v>
       </c>
       <c r="C80" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -10318,10 +10198,10 @@
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>890</v>
+        <v>454</v>
       </c>
       <c r="C81" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -10329,7 +10209,7 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>437</v>
+        <v>455</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
@@ -10340,7 +10220,7 @@
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>438</v>
+        <v>456</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
@@ -10351,7 +10231,7 @@
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
@@ -10362,7 +10242,7 @@
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
@@ -10373,10 +10253,10 @@
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>909</v>
+        <v>459</v>
       </c>
       <c r="C86" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -10384,10 +10264,10 @@
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>910</v>
+        <v>460</v>
       </c>
       <c r="C87" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -10395,7 +10275,7 @@
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>441</v>
+        <v>461</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
@@ -10406,7 +10286,7 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>442</v>
+        <v>462</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
@@ -10417,7 +10297,7 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>443</v>
+        <v>463</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
@@ -10428,7 +10308,7 @@
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>444</v>
+        <v>464</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
@@ -10439,10 +10319,10 @@
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>891</v>
+        <v>465</v>
       </c>
       <c r="C92" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -10450,10 +10330,10 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>892</v>
+        <v>466</v>
       </c>
       <c r="C93" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -10461,7 +10341,7 @@
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>445</v>
+        <v>467</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
@@ -10472,7 +10352,7 @@
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>446</v>
+        <v>468</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
@@ -10483,7 +10363,7 @@
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>447</v>
+        <v>469</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
@@ -10494,7 +10374,7 @@
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>448</v>
+        <v>470</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
@@ -10505,10 +10385,10 @@
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>911</v>
+        <v>471</v>
       </c>
       <c r="C98" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -10516,10 +10396,10 @@
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>912</v>
+        <v>472</v>
       </c>
       <c r="C99" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -10527,7 +10407,7 @@
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>449</v>
+        <v>473</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
@@ -10538,7 +10418,7 @@
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>450</v>
+        <v>474</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
@@ -10549,7 +10429,7 @@
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>451</v>
+        <v>475</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
@@ -10560,7 +10440,7 @@
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>452</v>
+        <v>476</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
@@ -10571,10 +10451,10 @@
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>893</v>
+        <v>477</v>
       </c>
       <c r="C104" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -10582,10 +10462,10 @@
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>894</v>
+        <v>478</v>
       </c>
       <c r="C105" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -10593,7 +10473,7 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>453</v>
+        <v>479</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
@@ -10604,7 +10484,7 @@
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>454</v>
+        <v>480</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
@@ -10615,7 +10495,7 @@
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>455</v>
+        <v>573</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
@@ -10626,7 +10506,7 @@
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>456</v>
+        <v>574</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
@@ -10637,10 +10517,10 @@
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>913</v>
+        <v>575</v>
       </c>
       <c r="C110" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -10648,10 +10528,10 @@
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>914</v>
+        <v>576</v>
       </c>
       <c r="C111" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -10659,7 +10539,7 @@
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>457</v>
+        <v>577</v>
       </c>
       <c r="C112" t="s">
         <v>1</v>
@@ -10670,7 +10550,7 @@
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>458</v>
+        <v>578</v>
       </c>
       <c r="C113" t="s">
         <v>1</v>
@@ -10681,7 +10561,7 @@
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>459</v>
+        <v>579</v>
       </c>
       <c r="C114" t="s">
         <v>1</v>
@@ -10692,7 +10572,7 @@
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>460</v>
+        <v>580</v>
       </c>
       <c r="C115" t="s">
         <v>1</v>
@@ -10703,10 +10583,10 @@
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>895</v>
+        <v>581</v>
       </c>
       <c r="C116" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -10714,10 +10594,10 @@
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>896</v>
+        <v>582</v>
       </c>
       <c r="C117" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -10725,7 +10605,7 @@
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>461</v>
+        <v>583</v>
       </c>
       <c r="C118" t="s">
         <v>1</v>
@@ -10736,7 +10616,7 @@
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>462</v>
+        <v>584</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
@@ -10747,7 +10627,7 @@
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>463</v>
+        <v>585</v>
       </c>
       <c r="C120" t="s">
         <v>1</v>
@@ -10758,7 +10638,7 @@
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>464</v>
+        <v>586</v>
       </c>
       <c r="C121" t="s">
         <v>1</v>
@@ -10769,10 +10649,10 @@
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>915</v>
+        <v>587</v>
       </c>
       <c r="C122" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -10780,10 +10660,10 @@
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>916</v>
+        <v>588</v>
       </c>
       <c r="C123" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D123">
         <v>1</v>
@@ -10791,7 +10671,7 @@
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>465</v>
+        <v>589</v>
       </c>
       <c r="C124" t="s">
         <v>1</v>
@@ -10802,7 +10682,7 @@
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>466</v>
+        <v>590</v>
       </c>
       <c r="C125" t="s">
         <v>1</v>
@@ -10813,7 +10693,7 @@
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>467</v>
+        <v>591</v>
       </c>
       <c r="C126" t="s">
         <v>1</v>
@@ -10824,7 +10704,7 @@
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>468</v>
+        <v>592</v>
       </c>
       <c r="C127" t="s">
         <v>1</v>
@@ -10835,7 +10715,7 @@
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>897</v>
+        <v>814</v>
       </c>
       <c r="C128" t="s">
         <v>143</v>
@@ -10846,10 +10726,10 @@
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>898</v>
+        <v>835</v>
       </c>
       <c r="C129" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -10857,7 +10737,7 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>469</v>
+        <v>836</v>
       </c>
       <c r="C130" t="s">
         <v>1</v>
@@ -10868,7 +10748,7 @@
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>470</v>
+        <v>837</v>
       </c>
       <c r="C131" t="s">
         <v>1</v>
@@ -10879,7 +10759,7 @@
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>471</v>
+        <v>838</v>
       </c>
       <c r="C132" t="s">
         <v>1</v>
@@ -10890,7 +10770,7 @@
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>472</v>
+        <v>840</v>
       </c>
       <c r="C133" t="s">
         <v>1</v>
@@ -10901,7 +10781,7 @@
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>917</v>
+        <v>851</v>
       </c>
       <c r="C134" t="s">
         <v>143</v>
@@ -10912,7 +10792,7 @@
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>918</v>
+        <v>898</v>
       </c>
       <c r="C135" t="s">
         <v>143</v>
@@ -10923,10 +10803,10 @@
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>473</v>
+        <v>899</v>
       </c>
       <c r="C136" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -10934,10 +10814,10 @@
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>474</v>
+        <v>900</v>
       </c>
       <c r="C137" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -10945,10 +10825,10 @@
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>475</v>
+        <v>901</v>
       </c>
       <c r="C138" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -10956,10 +10836,10 @@
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>476</v>
+        <v>902</v>
       </c>
       <c r="C139" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D139">
         <v>1</v>
@@ -10967,7 +10847,7 @@
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
       <c r="C140" t="s">
         <v>143</v>
@@ -10978,7 +10858,7 @@
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="C141" t="s">
         <v>143</v>
@@ -10989,10 +10869,10 @@
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>477</v>
+        <v>905</v>
       </c>
       <c r="C142" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D142">
         <v>1</v>
@@ -11000,10 +10880,10 @@
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>478</v>
+        <v>906</v>
       </c>
       <c r="C143" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -11011,452 +10891,12 @@
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>479</v>
+        <v>907</v>
       </c>
       <c r="C144" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="D144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B145" t="s">
-        <v>480</v>
-      </c>
-      <c r="C145" t="s">
-        <v>1</v>
-      </c>
-      <c r="D145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
-        <v>919</v>
-      </c>
-      <c r="C146" t="s">
-        <v>143</v>
-      </c>
-      <c r="D146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B147" t="s">
-        <v>920</v>
-      </c>
-      <c r="C147" t="s">
-        <v>143</v>
-      </c>
-      <c r="D147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B148" t="s">
-        <v>573</v>
-      </c>
-      <c r="C148" t="s">
-        <v>1</v>
-      </c>
-      <c r="D148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B149" t="s">
-        <v>574</v>
-      </c>
-      <c r="C149" t="s">
-        <v>1</v>
-      </c>
-      <c r="D149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" t="s">
-        <v>575</v>
-      </c>
-      <c r="C150" t="s">
-        <v>1</v>
-      </c>
-      <c r="D150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" t="s">
-        <v>576</v>
-      </c>
-      <c r="C151" t="s">
-        <v>1</v>
-      </c>
-      <c r="D151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B152" t="s">
-        <v>577</v>
-      </c>
-      <c r="C152" t="s">
-        <v>1</v>
-      </c>
-      <c r="D152">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B153" t="s">
-        <v>578</v>
-      </c>
-      <c r="C153" t="s">
-        <v>1</v>
-      </c>
-      <c r="D153">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
-        <v>579</v>
-      </c>
-      <c r="C154" t="s">
-        <v>1</v>
-      </c>
-      <c r="D154">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B155" t="s">
-        <v>580</v>
-      </c>
-      <c r="C155" t="s">
-        <v>1</v>
-      </c>
-      <c r="D155">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
-        <v>581</v>
-      </c>
-      <c r="C156" t="s">
-        <v>1</v>
-      </c>
-      <c r="D156">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B157" t="s">
-        <v>582</v>
-      </c>
-      <c r="C157" t="s">
-        <v>1</v>
-      </c>
-      <c r="D157">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B158" t="s">
-        <v>583</v>
-      </c>
-      <c r="C158" t="s">
-        <v>1</v>
-      </c>
-      <c r="D158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
-        <v>584</v>
-      </c>
-      <c r="C159" t="s">
-        <v>1</v>
-      </c>
-      <c r="D159">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
-        <v>585</v>
-      </c>
-      <c r="C160" t="s">
-        <v>1</v>
-      </c>
-      <c r="D160">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B161" t="s">
-        <v>586</v>
-      </c>
-      <c r="C161" t="s">
-        <v>1</v>
-      </c>
-      <c r="D161">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
-        <v>587</v>
-      </c>
-      <c r="C162" t="s">
-        <v>1</v>
-      </c>
-      <c r="D162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>588</v>
-      </c>
-      <c r="C163" t="s">
-        <v>1</v>
-      </c>
-      <c r="D163">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
-        <v>589</v>
-      </c>
-      <c r="C164" t="s">
-        <v>1</v>
-      </c>
-      <c r="D164">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
-        <v>590</v>
-      </c>
-      <c r="C165" t="s">
-        <v>1</v>
-      </c>
-      <c r="D165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B166" t="s">
-        <v>591</v>
-      </c>
-      <c r="C166" t="s">
-        <v>1</v>
-      </c>
-      <c r="D166">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B167" t="s">
-        <v>592</v>
-      </c>
-      <c r="C167" t="s">
-        <v>1</v>
-      </c>
-      <c r="D167">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
-        <v>814</v>
-      </c>
-      <c r="C168" t="s">
-        <v>143</v>
-      </c>
-      <c r="D168">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B169" t="s">
-        <v>835</v>
-      </c>
-      <c r="C169" t="s">
-        <v>1</v>
-      </c>
-      <c r="D169">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B170" t="s">
-        <v>836</v>
-      </c>
-      <c r="C170" t="s">
-        <v>1</v>
-      </c>
-      <c r="D170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
-        <v>837</v>
-      </c>
-      <c r="C171" t="s">
-        <v>1</v>
-      </c>
-      <c r="D171">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B172" t="s">
-        <v>838</v>
-      </c>
-      <c r="C172" t="s">
-        <v>1</v>
-      </c>
-      <c r="D172">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
-        <v>840</v>
-      </c>
-      <c r="C173" t="s">
-        <v>1</v>
-      </c>
-      <c r="D173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>851</v>
-      </c>
-      <c r="C174" t="s">
-        <v>143</v>
-      </c>
-      <c r="D174">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>938</v>
-      </c>
-      <c r="C175" t="s">
-        <v>143</v>
-      </c>
-      <c r="D175">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>939</v>
-      </c>
-      <c r="C176" t="s">
-        <v>143</v>
-      </c>
-      <c r="D176">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B177" t="s">
-        <v>940</v>
-      </c>
-      <c r="C177" t="s">
-        <v>143</v>
-      </c>
-      <c r="D177">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
-        <v>941</v>
-      </c>
-      <c r="C178" t="s">
-        <v>143</v>
-      </c>
-      <c r="D178">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>942</v>
-      </c>
-      <c r="C179" t="s">
-        <v>143</v>
-      </c>
-      <c r="D179">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
-        <v>943</v>
-      </c>
-      <c r="C180" t="s">
-        <v>143</v>
-      </c>
-      <c r="D180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>944</v>
-      </c>
-      <c r="C181" t="s">
-        <v>143</v>
-      </c>
-      <c r="D181">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>945</v>
-      </c>
-      <c r="C182" t="s">
-        <v>143</v>
-      </c>
-      <c r="D182">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B183" t="s">
-        <v>946</v>
-      </c>
-      <c r="C183" t="s">
-        <v>143</v>
-      </c>
-      <c r="D183">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
-        <v>947</v>
-      </c>
-      <c r="C184" t="s">
-        <v>143</v>
-      </c>
-      <c r="D184">
         <v>1</v>
       </c>
     </row>

</xml_diff>